<commit_message>
updated baadtvbt, syfafe, syvbt
</commit_message>
<xml_diff>
--- a/InputData/trans/SYFAFE/Start Year Fleet Avg Fuel Economy.xlsx
+++ b/InputData/trans/SYFAFE/Start Year Fleet Avg Fuel Economy.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25726"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26130"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\olivia\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Olivia Ashmoore\Documents\EPS_Models by Region\Canada\eps-canada\InputData\trans\SYFAFE\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9AD72FEC-19D8-4032-A3C6-2EBD7BDA5D5B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6CD4B245-DAB9-4B07-8FD7-37D70960E454}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="13590" yWindow="1005" windowWidth="15060" windowHeight="16395" tabRatio="919" firstSheet="6" activeTab="14" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="585" yWindow="390" windowWidth="14295" windowHeight="15930" tabRatio="919" firstSheet="12" activeTab="14" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="About" sheetId="1" r:id="rId1"/>
@@ -26,11 +26,13 @@
     <sheet name="Onroad Calcs" sheetId="44" r:id="rId11"/>
     <sheet name="Marine Energy Consumption" sheetId="45" r:id="rId12"/>
     <sheet name="marine calcs" sheetId="46" r:id="rId13"/>
-    <sheet name="SYFAFE-psgr" sheetId="23" r:id="rId14"/>
-    <sheet name="SYFAFE-frgt" sheetId="24" r:id="rId15"/>
+    <sheet name="rail calcs" sheetId="48" r:id="rId14"/>
+    <sheet name="Table 25_rail" sheetId="49" r:id="rId15"/>
+    <sheet name="SYFAFE-psgr" sheetId="23" r:id="rId16"/>
+    <sheet name="SYFAFE-frgt" sheetId="24" r:id="rId17"/>
   </sheets>
   <externalReferences>
-    <externalReference r:id="rId16"/>
+    <externalReference r:id="rId18"/>
   </externalReferences>
   <definedNames>
     <definedName name="btu_per_pj">About!$A$28</definedName>
@@ -39,28 +41,28 @@
     <definedName name="elec_share">'Fuel Efficiency Adjustments'!$B$6</definedName>
     <definedName name="Eno_TM" localSheetId="12">'[1]1997  Table 1a Modified'!#REF!</definedName>
     <definedName name="Eno_TM" localSheetId="11">'[1]1997  Table 1a Modified'!#REF!</definedName>
-    <definedName name="Eno_TM" localSheetId="14">'[1]1997  Table 1a Modified'!#REF!</definedName>
+    <definedName name="Eno_TM" localSheetId="16">'[1]1997  Table 1a Modified'!#REF!</definedName>
     <definedName name="Eno_TM">'[1]1997  Table 1a Modified'!#REF!</definedName>
     <definedName name="Eno_Tons" localSheetId="12">'[1]1997  Table 1a Modified'!#REF!</definedName>
     <definedName name="Eno_Tons" localSheetId="11">'[1]1997  Table 1a Modified'!#REF!</definedName>
-    <definedName name="Eno_Tons" localSheetId="14">'[1]1997  Table 1a Modified'!#REF!</definedName>
+    <definedName name="Eno_Tons" localSheetId="16">'[1]1997  Table 1a Modified'!#REF!</definedName>
     <definedName name="Eno_Tons">'[1]1997  Table 1a Modified'!#REF!</definedName>
     <definedName name="km_per_mile">About!$A$27</definedName>
     <definedName name="Sum_T2" localSheetId="12">'[1]1997  Table 1a Modified'!#REF!</definedName>
     <definedName name="Sum_T2" localSheetId="11">'[1]1997  Table 1a Modified'!#REF!</definedName>
-    <definedName name="Sum_T2" localSheetId="14">'[1]1997  Table 1a Modified'!#REF!</definedName>
+    <definedName name="Sum_T2" localSheetId="16">'[1]1997  Table 1a Modified'!#REF!</definedName>
     <definedName name="Sum_T2">'[1]1997  Table 1a Modified'!#REF!</definedName>
     <definedName name="Sum_TTM" localSheetId="12">'[1]1997  Table 1a Modified'!#REF!</definedName>
     <definedName name="Sum_TTM" localSheetId="11">'[1]1997  Table 1a Modified'!#REF!</definedName>
-    <definedName name="Sum_TTM" localSheetId="14">'[1]1997  Table 1a Modified'!#REF!</definedName>
+    <definedName name="Sum_TTM" localSheetId="16">'[1]1997  Table 1a Modified'!#REF!</definedName>
     <definedName name="Sum_TTM">'[1]1997  Table 1a Modified'!#REF!</definedName>
     <definedName name="ti_tbl_50" localSheetId="12">#REF!</definedName>
     <definedName name="ti_tbl_50" localSheetId="11">#REF!</definedName>
-    <definedName name="ti_tbl_50" localSheetId="14">#REF!</definedName>
+    <definedName name="ti_tbl_50" localSheetId="16">#REF!</definedName>
     <definedName name="ti_tbl_50">#REF!</definedName>
     <definedName name="ti_tbl_69" localSheetId="12">#REF!</definedName>
     <definedName name="ti_tbl_69" localSheetId="11">#REF!</definedName>
-    <definedName name="ti_tbl_69" localSheetId="14">#REF!</definedName>
+    <definedName name="ti_tbl_69" localSheetId="16">#REF!</definedName>
     <definedName name="ti_tbl_69">#REF!</definedName>
   </definedNames>
   <calcPr calcId="191028"/>
@@ -236,7 +238,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1443" uniqueCount="319">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1517" uniqueCount="336">
   <si>
     <t>SYFAFE Start Year Fleet Avg Fuel Economy</t>
   </si>
@@ -2649,6 +2651,122 @@
   <si>
     <t>Freight MDVs</t>
   </si>
+  <si>
+    <t>Table 25: Rail Transportation Secondary Energy Use and GHG Emissions by Region</t>
+  </si>
+  <si>
+    <r>
+      <t>Rail Transportation Energy Use</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <vertAlign val="superscript"/>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>1</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> (PJ)</t>
+    </r>
+  </si>
+  <si>
+    <t>Passenger Rail Transportation</t>
+  </si>
+  <si>
+    <t>Freight Rail Transportation</t>
+  </si>
+  <si>
+    <t>Passenger Rail Transportation Energy Intensity (MJ/Pkm)</t>
+  </si>
+  <si>
+    <t>Freight Rail Transportation Energy Intensity (MJ/Tkm)</t>
+  </si>
+  <si>
+    <r>
+      <t>Rail Transportation GHG Emissions</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <vertAlign val="superscript"/>
+        <sz val="10"/>
+        <color indexed="8"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>1</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color indexed="8"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> (Mt of CO</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <vertAlign val="subscript"/>
+        <sz val="10"/>
+        <color indexed="8"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>2</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color indexed="8"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>e)</t>
+    </r>
+  </si>
+  <si>
+    <t>Passenger Rail Transportation GHG Intensity (tonne/TJ)</t>
+  </si>
+  <si>
+    <t>Freight Rail Transportation GHG Intensity (tonne/TJ)</t>
+  </si>
+  <si>
+    <t>1) Rail transportation consumes only diesel fuel oil.</t>
+  </si>
+  <si>
+    <t>megajule to btu</t>
+  </si>
+  <si>
+    <t>btu per Tkm</t>
+  </si>
+  <si>
+    <t>btu per ton-mile</t>
+  </si>
+  <si>
+    <t>inverse (frgt-ton miles/btu)</t>
+  </si>
+  <si>
+    <t>km to miles</t>
+  </si>
+  <si>
+    <t>tonnes to tons</t>
+  </si>
+  <si>
+    <t>Units</t>
+  </si>
 </sst>
 </file>
 
@@ -2667,7 +2785,7 @@
     <numFmt numFmtId="171" formatCode="0.0000"/>
     <numFmt numFmtId="172" formatCode="0.0000E+00"/>
   </numFmts>
-  <fonts count="73">
+  <fonts count="77">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -3123,6 +3241,35 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <color indexed="8"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color indexed="8"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <vertAlign val="superscript"/>
+      <sz val="10"/>
+      <color indexed="8"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <vertAlign val="subscript"/>
+      <sz val="10"/>
+      <color indexed="8"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="33">
@@ -3768,7 +3915,7 @@
     <xf numFmtId="0" fontId="58" fillId="0" borderId="0"/>
     <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="99">
+  <cellXfs count="111">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -3913,9 +4060,39 @@
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="44" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="66" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="62" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="43" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="45" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="43" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="62" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="2" fontId="73" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="73" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="73" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="168" fontId="12" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="42" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="49" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="74" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="157">
     <cellStyle name="20% - Accent1 2" xfId="8" xr:uid="{00000000-0005-0000-0000-000000000000}"/>
@@ -4813,7 +4990,7 @@
 </file>
 
 <file path=xl/externalLinks/externalLink1.xml><?xml version="1.0" encoding="utf-8"?>
-<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
+<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xxl21="http://schemas.microsoft.com/office/spreadsheetml/2021/extlinks2021" mc:Ignorable="x14 xxl21">
   <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
     <sheetNames>
       <sheetName val="Rail shipments 93-97"/>
@@ -5803,10 +5980,10 @@
       <c r="AC2" s="32"/>
     </row>
     <row r="5" spans="1:32" ht="18" customHeight="1">
-      <c r="A5" s="98" t="s">
+      <c r="A5" s="96" t="s">
         <v>187</v>
       </c>
-      <c r="B5" s="98"/>
+      <c r="B5" s="96"/>
       <c r="C5" s="38"/>
       <c r="D5" s="38"/>
       <c r="E5" s="38"/>
@@ -7759,8 +7936,8 @@
       <c r="AF33" s="38"/>
     </row>
     <row r="34" spans="1:32" ht="14.65" customHeight="1">
-      <c r="A34" s="96"/>
-      <c r="B34" s="96"/>
+      <c r="A34" s="98"/>
+      <c r="B34" s="98"/>
       <c r="C34" s="15"/>
       <c r="D34" s="15"/>
       <c r="E34" s="15"/>
@@ -21936,16 +22113,42 @@
     </row>
   </sheetData>
   <mergeCells count="58">
-    <mergeCell ref="A204:B204"/>
-    <mergeCell ref="A216:B216"/>
-    <mergeCell ref="A218:B218"/>
-    <mergeCell ref="A219:B219"/>
-    <mergeCell ref="A160:B160"/>
-    <mergeCell ref="A173:B173"/>
-    <mergeCell ref="A185:B185"/>
-    <mergeCell ref="A188:B188"/>
-    <mergeCell ref="A190:B190"/>
-    <mergeCell ref="A191:B191"/>
+    <mergeCell ref="A34:B34"/>
+    <mergeCell ref="A5:B5"/>
+    <mergeCell ref="A6:B6"/>
+    <mergeCell ref="A7:B7"/>
+    <mergeCell ref="A8:B8"/>
+    <mergeCell ref="A9:B9"/>
+    <mergeCell ref="A10:B10"/>
+    <mergeCell ref="A11:B11"/>
+    <mergeCell ref="A12:B12"/>
+    <mergeCell ref="A21:B21"/>
+    <mergeCell ref="A29:B29"/>
+    <mergeCell ref="A32:B32"/>
+    <mergeCell ref="A79:B79"/>
+    <mergeCell ref="A35:B35"/>
+    <mergeCell ref="A44:B44"/>
+    <mergeCell ref="A52:B52"/>
+    <mergeCell ref="A54:B54"/>
+    <mergeCell ref="A55:B55"/>
+    <mergeCell ref="A56:B56"/>
+    <mergeCell ref="A57:B57"/>
+    <mergeCell ref="A58:B58"/>
+    <mergeCell ref="A59:B59"/>
+    <mergeCell ref="A68:B68"/>
+    <mergeCell ref="A76:B76"/>
+    <mergeCell ref="A125:B125"/>
+    <mergeCell ref="A81:B81"/>
+    <mergeCell ref="A82:B82"/>
+    <mergeCell ref="A91:B91"/>
+    <mergeCell ref="A99:B99"/>
+    <mergeCell ref="A101:B101"/>
+    <mergeCell ref="A102:B102"/>
+    <mergeCell ref="A103:B103"/>
+    <mergeCell ref="A104:B104"/>
+    <mergeCell ref="A105:B105"/>
+    <mergeCell ref="A106:B106"/>
+    <mergeCell ref="A116:B116"/>
     <mergeCell ref="A159:B159"/>
     <mergeCell ref="A128:B128"/>
     <mergeCell ref="A130:B130"/>
@@ -21958,42 +22161,16 @@
     <mergeCell ref="A156:B156"/>
     <mergeCell ref="A157:B157"/>
     <mergeCell ref="A158:B158"/>
-    <mergeCell ref="A125:B125"/>
-    <mergeCell ref="A81:B81"/>
-    <mergeCell ref="A82:B82"/>
-    <mergeCell ref="A91:B91"/>
-    <mergeCell ref="A99:B99"/>
-    <mergeCell ref="A101:B101"/>
-    <mergeCell ref="A102:B102"/>
-    <mergeCell ref="A103:B103"/>
-    <mergeCell ref="A104:B104"/>
-    <mergeCell ref="A105:B105"/>
-    <mergeCell ref="A106:B106"/>
-    <mergeCell ref="A116:B116"/>
-    <mergeCell ref="A79:B79"/>
-    <mergeCell ref="A35:B35"/>
-    <mergeCell ref="A44:B44"/>
-    <mergeCell ref="A52:B52"/>
-    <mergeCell ref="A54:B54"/>
-    <mergeCell ref="A55:B55"/>
-    <mergeCell ref="A56:B56"/>
-    <mergeCell ref="A57:B57"/>
-    <mergeCell ref="A58:B58"/>
-    <mergeCell ref="A59:B59"/>
-    <mergeCell ref="A68:B68"/>
-    <mergeCell ref="A76:B76"/>
-    <mergeCell ref="A34:B34"/>
-    <mergeCell ref="A5:B5"/>
-    <mergeCell ref="A6:B6"/>
-    <mergeCell ref="A7:B7"/>
-    <mergeCell ref="A8:B8"/>
-    <mergeCell ref="A9:B9"/>
-    <mergeCell ref="A10:B10"/>
-    <mergeCell ref="A11:B11"/>
-    <mergeCell ref="A12:B12"/>
-    <mergeCell ref="A21:B21"/>
-    <mergeCell ref="A29:B29"/>
-    <mergeCell ref="A32:B32"/>
+    <mergeCell ref="A204:B204"/>
+    <mergeCell ref="A216:B216"/>
+    <mergeCell ref="A218:B218"/>
+    <mergeCell ref="A219:B219"/>
+    <mergeCell ref="A160:B160"/>
+    <mergeCell ref="A173:B173"/>
+    <mergeCell ref="A185:B185"/>
+    <mergeCell ref="A188:B188"/>
+    <mergeCell ref="A190:B190"/>
+    <mergeCell ref="A191:B191"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -32082,14 +32259,3850 @@
 </file>
 
 <file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BB40D0D7-9817-46EB-AC27-A9B7F4096646}">
+  <sheetPr>
+    <tabColor theme="9"/>
+  </sheetPr>
+  <dimension ref="B2:C19"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D27" sqref="D27"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="2" max="2" width="62.85546875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="2:3">
+      <c r="B2" s="100" t="s">
+        <v>323</v>
+      </c>
+      <c r="C2" s="34">
+        <f>'Table 25_rail'!V38</f>
+        <v>1.3182579999999999</v>
+      </c>
+    </row>
+    <row r="3" spans="2:3">
+      <c r="B3" s="100" t="s">
+        <v>324</v>
+      </c>
+      <c r="C3" s="34">
+        <f>'Table 25_rail'!V39</f>
+        <v>0.21271200000000001</v>
+      </c>
+    </row>
+    <row r="5" spans="2:3">
+      <c r="B5" s="1" t="s">
+        <v>335</v>
+      </c>
+    </row>
+    <row r="6" spans="2:3">
+      <c r="B6" t="s">
+        <v>329</v>
+      </c>
+      <c r="C6">
+        <v>947.81700000000001</v>
+      </c>
+    </row>
+    <row r="7" spans="2:3">
+      <c r="B7" t="s">
+        <v>333</v>
+      </c>
+      <c r="C7">
+        <v>0.62137100000000001</v>
+      </c>
+    </row>
+    <row r="8" spans="2:3">
+      <c r="B8" t="s">
+        <v>334</v>
+      </c>
+      <c r="C8">
+        <v>0.90718500000000002</v>
+      </c>
+    </row>
+    <row r="10" spans="2:3">
+      <c r="B10" s="99" t="s">
+        <v>324</v>
+      </c>
+      <c r="C10" s="34">
+        <f>C3</f>
+        <v>0.21271200000000001</v>
+      </c>
+    </row>
+    <row r="11" spans="2:3">
+      <c r="B11" t="s">
+        <v>330</v>
+      </c>
+      <c r="C11">
+        <f>C10*C6</f>
+        <v>201.61204970400001</v>
+      </c>
+    </row>
+    <row r="12" spans="2:3">
+      <c r="B12" t="s">
+        <v>331</v>
+      </c>
+      <c r="C12">
+        <f>C11/C7/C8</f>
+        <v>357.65940012232835</v>
+      </c>
+    </row>
+    <row r="13" spans="2:3">
+      <c r="B13" t="s">
+        <v>332</v>
+      </c>
+      <c r="C13" s="9">
+        <f>1/C12</f>
+        <v>2.7959561517409449E-3</v>
+      </c>
+    </row>
+    <row r="16" spans="2:3">
+      <c r="B16" s="100" t="s">
+        <v>323</v>
+      </c>
+      <c r="C16" s="34">
+        <f>C2</f>
+        <v>1.3182579999999999</v>
+      </c>
+    </row>
+    <row r="17" spans="2:3">
+      <c r="B17" t="s">
+        <v>330</v>
+      </c>
+      <c r="C17">
+        <f>C16*C6</f>
+        <v>1249.467342786</v>
+      </c>
+    </row>
+    <row r="18" spans="2:3">
+      <c r="B18" t="s">
+        <v>331</v>
+      </c>
+      <c r="C18">
+        <f>C17/C7/C8</f>
+        <v>2216.5527355601012</v>
+      </c>
+    </row>
+    <row r="19" spans="2:3">
+      <c r="B19" t="s">
+        <v>332</v>
+      </c>
+      <c r="C19" s="9">
+        <f>1/C18</f>
+        <v>4.511510075790323E-4</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1C4EC087-1172-40CE-90A4-CF79C4572982}">
+  <dimension ref="A1:V72"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="W35" sqref="W35"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="2" max="2" width="41.42578125" style="105" customWidth="1"/>
+    <col min="3" max="21" width="0" hidden="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:22" ht="15.75">
+      <c r="A1" s="21" t="s">
+        <v>188</v>
+      </c>
+      <c r="C1" s="7"/>
+      <c r="D1" s="7"/>
+      <c r="E1" s="7"/>
+    </row>
+    <row r="2" spans="1:22" ht="15.75">
+      <c r="A2" s="21" t="s">
+        <v>319</v>
+      </c>
+      <c r="B2" s="106"/>
+      <c r="C2" s="18"/>
+      <c r="D2" s="18"/>
+      <c r="E2" s="18"/>
+      <c r="F2" s="19"/>
+      <c r="G2" s="19"/>
+      <c r="H2" s="19"/>
+      <c r="I2" s="19"/>
+      <c r="J2" s="19"/>
+      <c r="K2" s="19"/>
+      <c r="L2" s="19"/>
+      <c r="M2" s="19"/>
+      <c r="N2" s="19"/>
+      <c r="O2" s="19"/>
+      <c r="P2" s="19"/>
+      <c r="Q2" s="19"/>
+      <c r="R2" s="19"/>
+      <c r="S2" s="19"/>
+      <c r="T2" s="19"/>
+      <c r="U2" s="19"/>
+      <c r="V2" s="19"/>
+    </row>
+    <row r="5" spans="1:22">
+      <c r="C5" s="33">
+        <v>2000</v>
+      </c>
+      <c r="D5" s="33">
+        <v>2001</v>
+      </c>
+      <c r="E5" s="33">
+        <v>2002</v>
+      </c>
+      <c r="F5" s="33">
+        <v>2003</v>
+      </c>
+      <c r="G5" s="33">
+        <v>2004</v>
+      </c>
+      <c r="H5" s="33">
+        <v>2005</v>
+      </c>
+      <c r="I5" s="33">
+        <v>2006</v>
+      </c>
+      <c r="J5" s="33">
+        <v>2007</v>
+      </c>
+      <c r="K5" s="33">
+        <v>2008</v>
+      </c>
+      <c r="L5" s="33">
+        <v>2009</v>
+      </c>
+      <c r="M5" s="33">
+        <v>2010</v>
+      </c>
+      <c r="N5" s="33">
+        <v>2011</v>
+      </c>
+      <c r="O5" s="33">
+        <v>2012</v>
+      </c>
+      <c r="P5" s="33">
+        <v>2013</v>
+      </c>
+      <c r="Q5" s="33">
+        <v>2014</v>
+      </c>
+      <c r="R5" s="33">
+        <v>2015</v>
+      </c>
+      <c r="S5" s="33">
+        <v>2016</v>
+      </c>
+      <c r="T5" s="33">
+        <v>2017</v>
+      </c>
+      <c r="U5" s="33">
+        <v>2018</v>
+      </c>
+      <c r="V5" s="33">
+        <v>2019</v>
+      </c>
+    </row>
+    <row r="7" spans="1:22">
+      <c r="A7" s="15"/>
+      <c r="B7" s="75" t="s">
+        <v>320</v>
+      </c>
+      <c r="C7" s="65">
+        <v>84.48</v>
+      </c>
+      <c r="D7" s="65">
+        <v>83.701999999999998</v>
+      </c>
+      <c r="E7" s="65">
+        <v>76.23</v>
+      </c>
+      <c r="F7" s="65">
+        <v>76.960999999999999</v>
+      </c>
+      <c r="G7" s="65">
+        <v>79.138999999999996</v>
+      </c>
+      <c r="H7" s="65">
+        <v>84.325999999999993</v>
+      </c>
+      <c r="I7" s="65">
+        <v>88.275999999999996</v>
+      </c>
+      <c r="J7" s="65">
+        <v>94.558000000000007</v>
+      </c>
+      <c r="K7" s="65">
+        <v>99.834999999999994</v>
+      </c>
+      <c r="L7" s="65">
+        <v>85.356999999999999</v>
+      </c>
+      <c r="M7" s="65">
+        <v>83.724999999999994</v>
+      </c>
+      <c r="N7" s="65">
+        <v>94.36</v>
+      </c>
+      <c r="O7" s="65">
+        <v>96.578000000000003</v>
+      </c>
+      <c r="P7" s="65">
+        <v>93.05</v>
+      </c>
+      <c r="Q7" s="65">
+        <v>95.406000000000006</v>
+      </c>
+      <c r="R7" s="65">
+        <v>90.855999999999995</v>
+      </c>
+      <c r="S7" s="65">
+        <v>83.477000000000004</v>
+      </c>
+      <c r="T7" s="65">
+        <v>95.518000000000001</v>
+      </c>
+      <c r="U7" s="65">
+        <v>97.563999999999993</v>
+      </c>
+      <c r="V7" s="65">
+        <v>98.284999999999997</v>
+      </c>
+    </row>
+    <row r="8" spans="1:22">
+      <c r="B8" s="107" t="s">
+        <v>321</v>
+      </c>
+      <c r="C8" s="101">
+        <v>2.9738790000000002</v>
+      </c>
+      <c r="D8" s="101">
+        <v>2.9605899999999998</v>
+      </c>
+      <c r="E8" s="101">
+        <v>2.7514850000000002</v>
+      </c>
+      <c r="F8" s="101">
+        <v>2.6077520000000001</v>
+      </c>
+      <c r="G8" s="101">
+        <v>2.5421640000000001</v>
+      </c>
+      <c r="H8" s="101">
+        <v>2.6696439999999999</v>
+      </c>
+      <c r="I8" s="101">
+        <v>2.6993649999999998</v>
+      </c>
+      <c r="J8" s="101">
+        <v>2.8065530000000001</v>
+      </c>
+      <c r="K8" s="101">
+        <v>3.1555629999999999</v>
+      </c>
+      <c r="L8" s="101">
+        <v>2.9977499999999999</v>
+      </c>
+      <c r="M8" s="101">
+        <v>2.4749439999999998</v>
+      </c>
+      <c r="N8" s="101">
+        <v>2.7665929999999999</v>
+      </c>
+      <c r="O8" s="101">
+        <v>2.3815270000000002</v>
+      </c>
+      <c r="P8" s="101">
+        <v>2.1025550000000002</v>
+      </c>
+      <c r="Q8" s="101">
+        <v>1.9880899999999999</v>
+      </c>
+      <c r="R8" s="101">
+        <v>2.0039169999999999</v>
+      </c>
+      <c r="S8" s="101">
+        <v>2.0251960000000002</v>
+      </c>
+      <c r="T8" s="101">
+        <v>2.2895620000000001</v>
+      </c>
+      <c r="U8" s="101">
+        <v>2.237285</v>
+      </c>
+      <c r="V8" s="101">
+        <v>2.2928009999999999</v>
+      </c>
+    </row>
+    <row r="9" spans="1:22">
+      <c r="B9" s="107" t="s">
+        <v>322</v>
+      </c>
+      <c r="C9" s="101">
+        <v>81.506120999999993</v>
+      </c>
+      <c r="D9" s="101">
+        <v>80.741410000000002</v>
+      </c>
+      <c r="E9" s="101">
+        <v>73.478515000000002</v>
+      </c>
+      <c r="F9" s="101">
+        <v>74.353247999999994</v>
+      </c>
+      <c r="G9" s="101">
+        <v>76.596835999999996</v>
+      </c>
+      <c r="H9" s="101">
+        <v>81.656356000000002</v>
+      </c>
+      <c r="I9" s="101">
+        <v>85.576634999999996</v>
+      </c>
+      <c r="J9" s="101">
+        <v>91.751446999999999</v>
+      </c>
+      <c r="K9" s="101">
+        <v>96.679436999999993</v>
+      </c>
+      <c r="L9" s="101">
+        <v>82.359250000000003</v>
+      </c>
+      <c r="M9" s="101">
+        <v>81.250056000000001</v>
+      </c>
+      <c r="N9" s="101">
+        <v>91.593406999999999</v>
+      </c>
+      <c r="O9" s="101">
+        <v>94.196472999999997</v>
+      </c>
+      <c r="P9" s="101">
+        <v>90.947445000000002</v>
+      </c>
+      <c r="Q9" s="101">
+        <v>93.417910000000006</v>
+      </c>
+      <c r="R9" s="101">
+        <v>88.852082999999993</v>
+      </c>
+      <c r="S9" s="101">
+        <v>81.451803999999996</v>
+      </c>
+      <c r="T9" s="101">
+        <v>93.228437999999997</v>
+      </c>
+      <c r="U9" s="101">
+        <v>95.326714999999993</v>
+      </c>
+      <c r="V9" s="101">
+        <v>95.992198999999999</v>
+      </c>
+    </row>
+    <row r="10" spans="1:22">
+      <c r="B10" s="108" t="s">
+        <v>200</v>
+      </c>
+      <c r="C10" s="101"/>
+      <c r="D10" s="101"/>
+      <c r="E10" s="101"/>
+      <c r="F10" s="101"/>
+      <c r="G10" s="101"/>
+      <c r="H10" s="101"/>
+      <c r="I10" s="101"/>
+      <c r="J10" s="101"/>
+      <c r="K10" s="101"/>
+      <c r="L10" s="101"/>
+      <c r="M10" s="101"/>
+      <c r="N10" s="101"/>
+      <c r="O10" s="101"/>
+      <c r="P10" s="101"/>
+      <c r="Q10" s="101"/>
+      <c r="R10" s="101"/>
+      <c r="S10" s="101"/>
+      <c r="T10" s="101"/>
+      <c r="U10" s="101"/>
+      <c r="V10" s="101"/>
+    </row>
+    <row r="11" spans="1:22">
+      <c r="B11" s="107" t="s">
+        <v>201</v>
+      </c>
+      <c r="C11" s="101">
+        <v>0</v>
+      </c>
+      <c r="D11" s="101">
+        <v>0</v>
+      </c>
+      <c r="E11" s="101">
+        <v>0</v>
+      </c>
+      <c r="F11" s="101">
+        <v>0</v>
+      </c>
+      <c r="G11" s="101">
+        <v>0</v>
+      </c>
+      <c r="H11" s="101">
+        <v>0</v>
+      </c>
+      <c r="I11" s="101">
+        <v>0</v>
+      </c>
+      <c r="J11" s="101">
+        <v>0</v>
+      </c>
+      <c r="K11" s="101">
+        <v>0</v>
+      </c>
+      <c r="L11" s="101">
+        <v>0</v>
+      </c>
+      <c r="M11" s="101">
+        <v>0</v>
+      </c>
+      <c r="N11" s="101">
+        <v>0</v>
+      </c>
+      <c r="O11" s="101">
+        <v>0</v>
+      </c>
+      <c r="P11" s="101">
+        <v>0</v>
+      </c>
+      <c r="Q11" s="101">
+        <v>0</v>
+      </c>
+      <c r="R11" s="101">
+        <v>0</v>
+      </c>
+      <c r="S11" s="101">
+        <v>0</v>
+      </c>
+      <c r="T11" s="101">
+        <v>0</v>
+      </c>
+      <c r="U11" s="101">
+        <v>0</v>
+      </c>
+      <c r="V11" s="101">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:22">
+      <c r="B12" s="107" t="s">
+        <v>202</v>
+      </c>
+      <c r="C12" s="101">
+        <v>0</v>
+      </c>
+      <c r="D12" s="101">
+        <v>0</v>
+      </c>
+      <c r="E12" s="101">
+        <v>0</v>
+      </c>
+      <c r="F12" s="101">
+        <v>0</v>
+      </c>
+      <c r="G12" s="101">
+        <v>0</v>
+      </c>
+      <c r="H12" s="101">
+        <v>0</v>
+      </c>
+      <c r="I12" s="101">
+        <v>0</v>
+      </c>
+      <c r="J12" s="101">
+        <v>0</v>
+      </c>
+      <c r="K12" s="101">
+        <v>0</v>
+      </c>
+      <c r="L12" s="101">
+        <v>0</v>
+      </c>
+      <c r="M12" s="101">
+        <v>0</v>
+      </c>
+      <c r="N12" s="101">
+        <v>0</v>
+      </c>
+      <c r="O12" s="101">
+        <v>0</v>
+      </c>
+      <c r="P12" s="101">
+        <v>0</v>
+      </c>
+      <c r="Q12" s="101">
+        <v>0</v>
+      </c>
+      <c r="R12" s="101">
+        <v>0</v>
+      </c>
+      <c r="S12" s="101">
+        <v>0</v>
+      </c>
+      <c r="T12" s="101">
+        <v>0</v>
+      </c>
+      <c r="U12" s="101">
+        <v>0</v>
+      </c>
+      <c r="V12" s="101">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:22">
+      <c r="B13" s="107" t="s">
+        <v>203</v>
+      </c>
+      <c r="C13" s="101">
+        <v>0.94299999999999995</v>
+      </c>
+      <c r="D13" s="101">
+        <v>0.88500000000000001</v>
+      </c>
+      <c r="E13" s="101">
+        <v>0.99</v>
+      </c>
+      <c r="F13" s="101">
+        <v>2.1080000000000001</v>
+      </c>
+      <c r="G13" s="101">
+        <v>1.5049999999999999</v>
+      </c>
+      <c r="H13" s="101">
+        <v>1.47</v>
+      </c>
+      <c r="I13" s="101">
+        <v>1.3360000000000001</v>
+      </c>
+      <c r="J13" s="101">
+        <v>1.9830000000000001</v>
+      </c>
+      <c r="K13" s="101">
+        <v>1.776</v>
+      </c>
+      <c r="L13" s="101">
+        <v>1.4750000000000001</v>
+      </c>
+      <c r="M13" s="101">
+        <v>1.748</v>
+      </c>
+      <c r="N13" s="101">
+        <v>2.1749999999999998</v>
+      </c>
+      <c r="O13" s="101">
+        <v>1.6759999999999999</v>
+      </c>
+      <c r="P13" s="101">
+        <v>1.337</v>
+      </c>
+      <c r="Q13" s="101">
+        <v>1.3859999999999999</v>
+      </c>
+      <c r="R13" s="101">
+        <v>1.5109999999999999</v>
+      </c>
+      <c r="S13" s="101">
+        <v>1.5269999999999999</v>
+      </c>
+      <c r="T13" s="101">
+        <v>1.9379999999999999</v>
+      </c>
+      <c r="U13" s="101">
+        <v>2.0830000000000002</v>
+      </c>
+      <c r="V13" s="101">
+        <v>2.028</v>
+      </c>
+    </row>
+    <row r="14" spans="1:22">
+      <c r="B14" s="107" t="s">
+        <v>204</v>
+      </c>
+      <c r="C14" s="101">
+        <v>2.9860000000000002</v>
+      </c>
+      <c r="D14" s="101">
+        <v>3.3239999999999998</v>
+      </c>
+      <c r="E14" s="101">
+        <v>3.3090000000000002</v>
+      </c>
+      <c r="F14" s="101">
+        <v>3.6</v>
+      </c>
+      <c r="G14" s="101">
+        <v>3.7290000000000001</v>
+      </c>
+      <c r="H14" s="101">
+        <v>3.6429999999999998</v>
+      </c>
+      <c r="I14" s="101">
+        <v>3.621</v>
+      </c>
+      <c r="J14" s="101">
+        <v>3.6589999999999998</v>
+      </c>
+      <c r="K14" s="101">
+        <v>3.1459999999999999</v>
+      </c>
+      <c r="L14" s="101">
+        <v>3.2330000000000001</v>
+      </c>
+      <c r="M14" s="101">
+        <v>3.919</v>
+      </c>
+      <c r="N14" s="101">
+        <v>3.7069999999999999</v>
+      </c>
+      <c r="O14" s="101">
+        <v>3.4940000000000002</v>
+      </c>
+      <c r="P14" s="101">
+        <v>2.5339999999999998</v>
+      </c>
+      <c r="Q14" s="101">
+        <v>2.6139999999999999</v>
+      </c>
+      <c r="R14" s="101">
+        <v>2.194</v>
+      </c>
+      <c r="S14" s="101">
+        <v>2.0449999999999999</v>
+      </c>
+      <c r="T14" s="101">
+        <v>2.0129999999999999</v>
+      </c>
+      <c r="U14" s="101">
+        <v>2.044</v>
+      </c>
+      <c r="V14" s="101">
+        <v>1.929</v>
+      </c>
+    </row>
+    <row r="15" spans="1:22">
+      <c r="B15" s="109" t="s">
+        <v>205</v>
+      </c>
+      <c r="C15" s="101">
+        <v>10.317</v>
+      </c>
+      <c r="D15" s="101">
+        <v>9.6929999999999996</v>
+      </c>
+      <c r="E15" s="101">
+        <v>9.5549999999999997</v>
+      </c>
+      <c r="F15" s="101">
+        <v>9.4930000000000003</v>
+      </c>
+      <c r="G15" s="101">
+        <v>10.393000000000001</v>
+      </c>
+      <c r="H15" s="101">
+        <v>9.0340000000000007</v>
+      </c>
+      <c r="I15" s="101">
+        <v>9.8160000000000007</v>
+      </c>
+      <c r="J15" s="101">
+        <v>11.282999999999999</v>
+      </c>
+      <c r="K15" s="101">
+        <v>11.382999999999999</v>
+      </c>
+      <c r="L15" s="101">
+        <v>11.846</v>
+      </c>
+      <c r="M15" s="101">
+        <v>10.804</v>
+      </c>
+      <c r="N15" s="101">
+        <v>11.39</v>
+      </c>
+      <c r="O15" s="101">
+        <v>11.891</v>
+      </c>
+      <c r="P15" s="101">
+        <v>11.1</v>
+      </c>
+      <c r="Q15" s="101">
+        <v>9.9130000000000003</v>
+      </c>
+      <c r="R15" s="101">
+        <v>8.7059999999999995</v>
+      </c>
+      <c r="S15" s="101">
+        <v>8.5950000000000006</v>
+      </c>
+      <c r="T15" s="101">
+        <v>7.931</v>
+      </c>
+      <c r="U15" s="101">
+        <v>8.8879999999999999</v>
+      </c>
+      <c r="V15" s="101">
+        <v>8.1530000000000005</v>
+      </c>
+    </row>
+    <row r="16" spans="1:22">
+      <c r="B16" s="109" t="s">
+        <v>206</v>
+      </c>
+      <c r="C16" s="101">
+        <v>21.381</v>
+      </c>
+      <c r="D16" s="101">
+        <v>20.234000000000002</v>
+      </c>
+      <c r="E16" s="101">
+        <v>18.707999999999998</v>
+      </c>
+      <c r="F16" s="101">
+        <v>16.413</v>
+      </c>
+      <c r="G16" s="101">
+        <v>18.513999999999999</v>
+      </c>
+      <c r="H16" s="101">
+        <v>19.878</v>
+      </c>
+      <c r="I16" s="101">
+        <v>18.856000000000002</v>
+      </c>
+      <c r="J16" s="101">
+        <v>19.640999999999998</v>
+      </c>
+      <c r="K16" s="101">
+        <v>19.617999999999999</v>
+      </c>
+      <c r="L16" s="101">
+        <v>14.723000000000001</v>
+      </c>
+      <c r="M16" s="101">
+        <v>16.053999999999998</v>
+      </c>
+      <c r="N16" s="101">
+        <v>16.920999999999999</v>
+      </c>
+      <c r="O16" s="101">
+        <v>15.875</v>
+      </c>
+      <c r="P16" s="101">
+        <v>16.82</v>
+      </c>
+      <c r="Q16" s="101">
+        <v>18.047000000000001</v>
+      </c>
+      <c r="R16" s="101">
+        <v>18.280999999999999</v>
+      </c>
+      <c r="S16" s="101">
+        <v>18.533999999999999</v>
+      </c>
+      <c r="T16" s="101">
+        <v>18.454999999999998</v>
+      </c>
+      <c r="U16" s="101">
+        <v>19.616</v>
+      </c>
+      <c r="V16" s="101">
+        <v>19.847000000000001</v>
+      </c>
+    </row>
+    <row r="17" spans="2:22">
+      <c r="B17" s="109" t="s">
+        <v>207</v>
+      </c>
+      <c r="C17" s="101">
+        <v>4.1070000000000002</v>
+      </c>
+      <c r="D17" s="101">
+        <v>3.1190000000000002</v>
+      </c>
+      <c r="E17" s="101">
+        <v>1.157</v>
+      </c>
+      <c r="F17" s="101">
+        <v>2.5939999999999999</v>
+      </c>
+      <c r="G17" s="101">
+        <v>3.758</v>
+      </c>
+      <c r="H17" s="101">
+        <v>3.8279999999999998</v>
+      </c>
+      <c r="I17" s="101">
+        <v>3.742</v>
+      </c>
+      <c r="J17" s="101">
+        <v>3.25</v>
+      </c>
+      <c r="K17" s="101">
+        <v>3.5209999999999999</v>
+      </c>
+      <c r="L17" s="101">
+        <v>6.6909999999999998</v>
+      </c>
+      <c r="M17" s="101">
+        <v>7.9880000000000004</v>
+      </c>
+      <c r="N17" s="101">
+        <v>8.84</v>
+      </c>
+      <c r="O17" s="101">
+        <v>7.883</v>
+      </c>
+      <c r="P17" s="101">
+        <v>7.2770000000000001</v>
+      </c>
+      <c r="Q17" s="101">
+        <v>8.3710000000000004</v>
+      </c>
+      <c r="R17" s="101">
+        <v>8.9930000000000003</v>
+      </c>
+      <c r="S17" s="101">
+        <v>8.4329999999999998</v>
+      </c>
+      <c r="T17" s="101">
+        <v>10.256</v>
+      </c>
+      <c r="U17" s="101">
+        <v>11.247999999999999</v>
+      </c>
+      <c r="V17" s="101">
+        <v>11.404999999999999</v>
+      </c>
+    </row>
+    <row r="18" spans="2:22">
+      <c r="B18" s="109" t="s">
+        <v>208</v>
+      </c>
+      <c r="C18" s="101">
+        <v>5.2380000000000004</v>
+      </c>
+      <c r="D18" s="101">
+        <v>3.887</v>
+      </c>
+      <c r="E18" s="101">
+        <v>3.141</v>
+      </c>
+      <c r="F18" s="101">
+        <v>2.4119999999999999</v>
+      </c>
+      <c r="G18" s="101">
+        <v>2.1749999999999998</v>
+      </c>
+      <c r="H18" s="101">
+        <v>5.2530000000000001</v>
+      </c>
+      <c r="I18" s="101">
+        <v>4.875</v>
+      </c>
+      <c r="J18" s="101">
+        <v>3.1819999999999999</v>
+      </c>
+      <c r="K18" s="101">
+        <v>6.0359999999999996</v>
+      </c>
+      <c r="L18" s="101">
+        <v>4.8529999999999998</v>
+      </c>
+      <c r="M18" s="101">
+        <v>8.8740000000000006</v>
+      </c>
+      <c r="N18" s="101">
+        <v>9.2189999999999994</v>
+      </c>
+      <c r="O18" s="101">
+        <v>7.1849999999999996</v>
+      </c>
+      <c r="P18" s="101">
+        <v>8.8759999999999994</v>
+      </c>
+      <c r="Q18" s="101">
+        <v>9.1669999999999998</v>
+      </c>
+      <c r="R18" s="101">
+        <v>10.241</v>
+      </c>
+      <c r="S18" s="101">
+        <v>9.9779999999999998</v>
+      </c>
+      <c r="T18" s="101">
+        <v>14.359</v>
+      </c>
+      <c r="U18" s="101">
+        <v>16.359000000000002</v>
+      </c>
+      <c r="V18" s="101">
+        <v>17.341000000000001</v>
+      </c>
+    </row>
+    <row r="19" spans="2:22">
+      <c r="B19" s="109" t="s">
+        <v>209</v>
+      </c>
+      <c r="C19" s="101">
+        <v>23.123999999999999</v>
+      </c>
+      <c r="D19" s="101">
+        <v>28.978999999999999</v>
+      </c>
+      <c r="E19" s="101">
+        <v>28.280999999999999</v>
+      </c>
+      <c r="F19" s="101">
+        <v>33.006</v>
+      </c>
+      <c r="G19" s="101">
+        <v>33.895000000000003</v>
+      </c>
+      <c r="H19" s="101">
+        <v>35.636000000000003</v>
+      </c>
+      <c r="I19" s="101">
+        <v>40.584000000000003</v>
+      </c>
+      <c r="J19" s="101">
+        <v>46.076999999999998</v>
+      </c>
+      <c r="K19" s="101">
+        <v>45.878</v>
+      </c>
+      <c r="L19" s="101">
+        <v>36.790999999999997</v>
+      </c>
+      <c r="M19" s="101">
+        <v>27.699000000000002</v>
+      </c>
+      <c r="N19" s="101">
+        <v>33.436</v>
+      </c>
+      <c r="O19" s="101">
+        <v>39.715000000000003</v>
+      </c>
+      <c r="P19" s="101">
+        <v>38.17</v>
+      </c>
+      <c r="Q19" s="101">
+        <v>37.219000000000001</v>
+      </c>
+      <c r="R19" s="101">
+        <v>32.264000000000003</v>
+      </c>
+      <c r="S19" s="101">
+        <v>24.152000000000001</v>
+      </c>
+      <c r="T19" s="101">
+        <v>26.402000000000001</v>
+      </c>
+      <c r="U19" s="101">
+        <v>24.359000000000002</v>
+      </c>
+      <c r="V19" s="101">
+        <v>24.867999999999999</v>
+      </c>
+    </row>
+    <row r="20" spans="2:22">
+      <c r="B20" s="109" t="s">
+        <v>210</v>
+      </c>
+      <c r="C20" s="101">
+        <v>16.384</v>
+      </c>
+      <c r="D20" s="101">
+        <v>13.581</v>
+      </c>
+      <c r="E20" s="101">
+        <v>11.089</v>
+      </c>
+      <c r="F20" s="101">
+        <v>7.335</v>
+      </c>
+      <c r="G20" s="101">
+        <v>5.17</v>
+      </c>
+      <c r="H20" s="101">
+        <v>5.5839999999999996</v>
+      </c>
+      <c r="I20" s="101">
+        <v>5.4459999999999997</v>
+      </c>
+      <c r="J20" s="101">
+        <v>5.4829999999999997</v>
+      </c>
+      <c r="K20" s="101">
+        <v>8.4770000000000003</v>
+      </c>
+      <c r="L20" s="101">
+        <v>5.7450000000000001</v>
+      </c>
+      <c r="M20" s="101">
+        <v>6.6390000000000002</v>
+      </c>
+      <c r="N20" s="101">
+        <v>8.6720000000000006</v>
+      </c>
+      <c r="O20" s="101">
+        <v>8.859</v>
+      </c>
+      <c r="P20" s="101">
+        <v>6.9359999999999999</v>
+      </c>
+      <c r="Q20" s="101">
+        <v>8.6890000000000001</v>
+      </c>
+      <c r="R20" s="101">
+        <v>8.6660000000000004</v>
+      </c>
+      <c r="S20" s="101">
+        <v>10.212999999999999</v>
+      </c>
+      <c r="T20" s="101">
+        <v>14.164</v>
+      </c>
+      <c r="U20" s="101">
+        <v>12.967000000000001</v>
+      </c>
+      <c r="V20" s="101">
+        <v>12.714</v>
+      </c>
+    </row>
+    <row r="21" spans="2:22">
+      <c r="B21" s="107"/>
+      <c r="C21" s="101"/>
+      <c r="D21" s="101"/>
+      <c r="E21" s="101"/>
+      <c r="F21" s="101"/>
+      <c r="G21" s="101"/>
+      <c r="H21" s="101"/>
+      <c r="I21" s="101"/>
+      <c r="J21" s="101"/>
+      <c r="K21" s="101"/>
+      <c r="L21" s="101"/>
+      <c r="M21" s="101"/>
+      <c r="N21" s="101"/>
+      <c r="O21" s="101"/>
+      <c r="P21" s="101"/>
+      <c r="Q21" s="101"/>
+      <c r="R21" s="101"/>
+      <c r="S21" s="101"/>
+      <c r="T21" s="101"/>
+      <c r="U21" s="101"/>
+      <c r="V21" s="101"/>
+    </row>
+    <row r="22" spans="2:22">
+      <c r="B22" s="108" t="s">
+        <v>192</v>
+      </c>
+      <c r="C22" s="101"/>
+      <c r="D22" s="101"/>
+      <c r="E22" s="101"/>
+      <c r="F22" s="101"/>
+      <c r="G22" s="101"/>
+      <c r="H22" s="101"/>
+      <c r="I22" s="101"/>
+      <c r="J22" s="101"/>
+      <c r="K22" s="101"/>
+      <c r="L22" s="101"/>
+      <c r="M22" s="101"/>
+      <c r="N22" s="101"/>
+      <c r="O22" s="101"/>
+      <c r="P22" s="101"/>
+      <c r="Q22" s="101"/>
+      <c r="R22" s="101"/>
+      <c r="S22" s="101"/>
+      <c r="T22" s="101"/>
+      <c r="U22" s="101"/>
+      <c r="V22" s="101"/>
+    </row>
+    <row r="23" spans="2:22">
+      <c r="B23" s="107" t="s">
+        <v>201</v>
+      </c>
+      <c r="C23" s="101">
+        <v>0</v>
+      </c>
+      <c r="D23" s="101">
+        <v>0</v>
+      </c>
+      <c r="E23" s="101">
+        <v>0</v>
+      </c>
+      <c r="F23" s="101">
+        <v>0</v>
+      </c>
+      <c r="G23" s="101">
+        <v>0</v>
+      </c>
+      <c r="H23" s="101">
+        <v>0</v>
+      </c>
+      <c r="I23" s="101">
+        <v>0</v>
+      </c>
+      <c r="J23" s="101">
+        <v>0</v>
+      </c>
+      <c r="K23" s="101">
+        <v>0</v>
+      </c>
+      <c r="L23" s="101">
+        <v>0</v>
+      </c>
+      <c r="M23" s="101">
+        <v>0</v>
+      </c>
+      <c r="N23" s="101">
+        <v>0</v>
+      </c>
+      <c r="O23" s="101">
+        <v>0</v>
+      </c>
+      <c r="P23" s="101">
+        <v>0</v>
+      </c>
+      <c r="Q23" s="101">
+        <v>0</v>
+      </c>
+      <c r="R23" s="101">
+        <v>0</v>
+      </c>
+      <c r="S23" s="101">
+        <v>0</v>
+      </c>
+      <c r="T23" s="101">
+        <v>0</v>
+      </c>
+      <c r="U23" s="101">
+        <v>0</v>
+      </c>
+      <c r="V23" s="101">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="2:22">
+      <c r="B24" s="107" t="s">
+        <v>202</v>
+      </c>
+      <c r="C24" s="101">
+        <v>0</v>
+      </c>
+      <c r="D24" s="101">
+        <v>0</v>
+      </c>
+      <c r="E24" s="101">
+        <v>0</v>
+      </c>
+      <c r="F24" s="101">
+        <v>0</v>
+      </c>
+      <c r="G24" s="101">
+        <v>0</v>
+      </c>
+      <c r="H24" s="101">
+        <v>0</v>
+      </c>
+      <c r="I24" s="101">
+        <v>0</v>
+      </c>
+      <c r="J24" s="101">
+        <v>0</v>
+      </c>
+      <c r="K24" s="101">
+        <v>0</v>
+      </c>
+      <c r="L24" s="101">
+        <v>0</v>
+      </c>
+      <c r="M24" s="101">
+        <v>0</v>
+      </c>
+      <c r="N24" s="101">
+        <v>0</v>
+      </c>
+      <c r="O24" s="101">
+        <v>0</v>
+      </c>
+      <c r="P24" s="101">
+        <v>0</v>
+      </c>
+      <c r="Q24" s="101">
+        <v>0</v>
+      </c>
+      <c r="R24" s="101">
+        <v>0</v>
+      </c>
+      <c r="S24" s="101">
+        <v>0</v>
+      </c>
+      <c r="T24" s="101">
+        <v>0</v>
+      </c>
+      <c r="U24" s="101">
+        <v>0</v>
+      </c>
+      <c r="V24" s="101">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="2:22">
+      <c r="B25" s="107" t="s">
+        <v>203</v>
+      </c>
+      <c r="C25" s="101">
+        <v>1.116241</v>
+      </c>
+      <c r="D25" s="101">
+        <v>1.0573220000000001</v>
+      </c>
+      <c r="E25" s="101">
+        <v>1.2987010000000001</v>
+      </c>
+      <c r="F25" s="101">
+        <v>2.7390500000000002</v>
+      </c>
+      <c r="G25" s="101">
+        <v>1.9017170000000001</v>
+      </c>
+      <c r="H25" s="101">
+        <v>1.7432350000000001</v>
+      </c>
+      <c r="I25" s="101">
+        <v>1.5134350000000001</v>
+      </c>
+      <c r="J25" s="101">
+        <v>2.0971259999999998</v>
+      </c>
+      <c r="K25" s="101">
+        <v>1.7789349999999999</v>
+      </c>
+      <c r="L25" s="101">
+        <v>1.7280359999999999</v>
+      </c>
+      <c r="M25" s="101">
+        <v>2.0877870000000001</v>
+      </c>
+      <c r="N25" s="101">
+        <v>2.305002</v>
+      </c>
+      <c r="O25" s="101">
+        <v>1.735385</v>
+      </c>
+      <c r="P25" s="101">
+        <v>1.4368620000000001</v>
+      </c>
+      <c r="Q25" s="101">
+        <v>1.452739</v>
+      </c>
+      <c r="R25" s="101">
+        <v>1.663071</v>
+      </c>
+      <c r="S25" s="101">
+        <v>1.8292459999999999</v>
+      </c>
+      <c r="T25" s="101">
+        <v>2.028937</v>
+      </c>
+      <c r="U25" s="101">
+        <v>2.1350090000000002</v>
+      </c>
+      <c r="V25" s="101">
+        <v>2.0633870000000001</v>
+      </c>
+    </row>
+    <row r="26" spans="2:22">
+      <c r="B26" s="107" t="s">
+        <v>204</v>
+      </c>
+      <c r="C26" s="101">
+        <v>3.534564</v>
+      </c>
+      <c r="D26" s="101">
+        <v>3.971231</v>
+      </c>
+      <c r="E26" s="101">
+        <v>4.3408110000000004</v>
+      </c>
+      <c r="F26" s="101">
+        <v>4.6776939999999998</v>
+      </c>
+      <c r="G26" s="101">
+        <v>4.7119619999999998</v>
+      </c>
+      <c r="H26" s="101">
+        <v>4.3201390000000002</v>
+      </c>
+      <c r="I26" s="101">
+        <v>4.1019079999999999</v>
+      </c>
+      <c r="J26" s="101">
+        <v>3.869583</v>
+      </c>
+      <c r="K26" s="101">
+        <v>3.1511990000000001</v>
+      </c>
+      <c r="L26" s="101">
+        <v>3.7876210000000001</v>
+      </c>
+      <c r="M26" s="101">
+        <v>4.6807999999999996</v>
+      </c>
+      <c r="N26" s="101">
+        <v>3.9285709999999998</v>
+      </c>
+      <c r="O26" s="101">
+        <v>3.617801</v>
+      </c>
+      <c r="P26" s="101">
+        <v>2.7232669999999999</v>
+      </c>
+      <c r="Q26" s="101">
+        <v>2.7398699999999998</v>
+      </c>
+      <c r="R26" s="101">
+        <v>2.4148100000000001</v>
+      </c>
+      <c r="S26" s="101">
+        <v>2.4497770000000001</v>
+      </c>
+      <c r="T26" s="101">
+        <v>2.107456</v>
+      </c>
+      <c r="U26" s="101">
+        <v>2.0950350000000002</v>
+      </c>
+      <c r="V26" s="101">
+        <v>1.9626600000000001</v>
+      </c>
+    </row>
+    <row r="27" spans="2:22">
+      <c r="B27" s="109" t="s">
+        <v>205</v>
+      </c>
+      <c r="C27" s="101">
+        <v>12.212358</v>
+      </c>
+      <c r="D27" s="101">
+        <v>11.580368</v>
+      </c>
+      <c r="E27" s="101">
+        <v>12.534435</v>
+      </c>
+      <c r="F27" s="101">
+        <v>12.334819</v>
+      </c>
+      <c r="G27" s="101">
+        <v>13.132588999999999</v>
+      </c>
+      <c r="H27" s="101">
+        <v>10.713184999999999</v>
+      </c>
+      <c r="I27" s="101">
+        <v>11.119669999999999</v>
+      </c>
+      <c r="J27" s="101">
+        <v>11.932359</v>
+      </c>
+      <c r="K27" s="101">
+        <v>11.401813000000001</v>
+      </c>
+      <c r="L27" s="101">
+        <v>13.878182000000001</v>
+      </c>
+      <c r="M27" s="101">
+        <v>12.90415</v>
+      </c>
+      <c r="N27" s="101">
+        <v>12.070793</v>
+      </c>
+      <c r="O27" s="101">
+        <v>12.312328000000001</v>
+      </c>
+      <c r="P27" s="101">
+        <v>11.929069999999999</v>
+      </c>
+      <c r="Q27" s="101">
+        <v>10.390332000000001</v>
+      </c>
+      <c r="R27" s="101">
+        <v>9.5821959999999997</v>
+      </c>
+      <c r="S27" s="101">
+        <v>10.296249</v>
+      </c>
+      <c r="T27" s="101">
+        <v>8.3031469999999992</v>
+      </c>
+      <c r="U27" s="101">
+        <v>9.1099180000000004</v>
+      </c>
+      <c r="V27" s="101">
+        <v>8.2952639999999995</v>
+      </c>
+    </row>
+    <row r="28" spans="2:22">
+      <c r="B28" s="109" t="s">
+        <v>206</v>
+      </c>
+      <c r="C28" s="101">
+        <v>25.308948999999998</v>
+      </c>
+      <c r="D28" s="101">
+        <v>24.173855</v>
+      </c>
+      <c r="E28" s="101">
+        <v>24.541519000000001</v>
+      </c>
+      <c r="F28" s="101">
+        <v>21.326385999999999</v>
+      </c>
+      <c r="G28" s="101">
+        <v>23.394280999999999</v>
+      </c>
+      <c r="H28" s="101">
+        <v>23.572800999999998</v>
+      </c>
+      <c r="I28" s="101">
+        <v>21.360278999999998</v>
+      </c>
+      <c r="J28" s="101">
+        <v>20.771377999999999</v>
+      </c>
+      <c r="K28" s="101">
+        <v>19.650423</v>
+      </c>
+      <c r="L28" s="101">
+        <v>17.248732</v>
+      </c>
+      <c r="M28" s="101">
+        <v>19.174679000000001</v>
+      </c>
+      <c r="N28" s="101">
+        <v>17.932386999999999</v>
+      </c>
+      <c r="O28" s="101">
+        <v>16.437491000000001</v>
+      </c>
+      <c r="P28" s="101">
+        <v>18.076302999999999</v>
+      </c>
+      <c r="Q28" s="101">
+        <v>18.916001000000001</v>
+      </c>
+      <c r="R28" s="101">
+        <v>20.120850999999998</v>
+      </c>
+      <c r="S28" s="101">
+        <v>22.202522999999999</v>
+      </c>
+      <c r="T28" s="101">
+        <v>19.320965999999999</v>
+      </c>
+      <c r="U28" s="101">
+        <v>20.105777</v>
+      </c>
+      <c r="V28" s="101">
+        <v>20.193314999999998</v>
+      </c>
+    </row>
+    <row r="29" spans="2:22">
+      <c r="B29" s="109" t="s">
+        <v>207</v>
+      </c>
+      <c r="C29" s="101">
+        <v>4.8615060000000003</v>
+      </c>
+      <c r="D29" s="101">
+        <v>3.726315</v>
+      </c>
+      <c r="E29" s="101">
+        <v>1.5177750000000001</v>
+      </c>
+      <c r="F29" s="101">
+        <v>3.3705379999999998</v>
+      </c>
+      <c r="G29" s="101">
+        <v>4.7486069999999998</v>
+      </c>
+      <c r="H29" s="101">
+        <v>4.5395250000000003</v>
+      </c>
+      <c r="I29" s="101">
+        <v>4.2389780000000004</v>
+      </c>
+      <c r="J29" s="101">
+        <v>3.4370440000000002</v>
+      </c>
+      <c r="K29" s="101">
+        <v>3.5268190000000001</v>
+      </c>
+      <c r="L29" s="101">
+        <v>7.8388419999999996</v>
+      </c>
+      <c r="M29" s="101">
+        <v>9.5407580000000003</v>
+      </c>
+      <c r="N29" s="101">
+        <v>9.3683759999999996</v>
+      </c>
+      <c r="O29" s="101">
+        <v>8.1623140000000003</v>
+      </c>
+      <c r="P29" s="101">
+        <v>7.8205270000000002</v>
+      </c>
+      <c r="Q29" s="101">
+        <v>8.7740810000000007</v>
+      </c>
+      <c r="R29" s="101">
+        <v>9.8980800000000002</v>
+      </c>
+      <c r="S29" s="101">
+        <v>10.102183999999999</v>
+      </c>
+      <c r="T29" s="101">
+        <v>10.737242999999999</v>
+      </c>
+      <c r="U29" s="101">
+        <v>11.528843</v>
+      </c>
+      <c r="V29" s="101">
+        <v>11.604009</v>
+      </c>
+    </row>
+    <row r="30" spans="2:22">
+      <c r="B30" s="109" t="s">
+        <v>208</v>
+      </c>
+      <c r="C30" s="101">
+        <v>6.2002839999999999</v>
+      </c>
+      <c r="D30" s="101">
+        <v>4.6438560000000004</v>
+      </c>
+      <c r="E30" s="101">
+        <v>4.120425</v>
+      </c>
+      <c r="F30" s="101">
+        <v>3.134055</v>
+      </c>
+      <c r="G30" s="101">
+        <v>2.748329</v>
+      </c>
+      <c r="H30" s="101">
+        <v>6.2293950000000002</v>
+      </c>
+      <c r="I30" s="101">
+        <v>5.5224520000000004</v>
+      </c>
+      <c r="J30" s="101">
+        <v>3.3651300000000002</v>
+      </c>
+      <c r="K30" s="101">
+        <v>6.0459759999999996</v>
+      </c>
+      <c r="L30" s="101">
+        <v>5.6855330000000004</v>
+      </c>
+      <c r="M30" s="101">
+        <v>10.598985000000001</v>
+      </c>
+      <c r="N30" s="101">
+        <v>9.7700300000000002</v>
+      </c>
+      <c r="O30" s="101">
+        <v>7.4395829999999998</v>
+      </c>
+      <c r="P30" s="101">
+        <v>9.5389579999999992</v>
+      </c>
+      <c r="Q30" s="101">
+        <v>9.6084099999999992</v>
+      </c>
+      <c r="R30" s="101">
+        <v>11.271682999999999</v>
+      </c>
+      <c r="S30" s="101">
+        <v>11.952992999999999</v>
+      </c>
+      <c r="T30" s="101">
+        <v>15.032769</v>
+      </c>
+      <c r="U30" s="101">
+        <v>16.767455000000002</v>
+      </c>
+      <c r="V30" s="101">
+        <v>17.643588000000001</v>
+      </c>
+    </row>
+    <row r="31" spans="2:22">
+      <c r="B31" s="109" t="s">
+        <v>209</v>
+      </c>
+      <c r="C31" s="101">
+        <v>27.372159</v>
+      </c>
+      <c r="D31" s="101">
+        <v>34.621634</v>
+      </c>
+      <c r="E31" s="101">
+        <v>37.099567</v>
+      </c>
+      <c r="F31" s="101">
+        <v>42.886657</v>
+      </c>
+      <c r="G31" s="101">
+        <v>42.829704999999997</v>
+      </c>
+      <c r="H31" s="101">
+        <v>42.259801000000003</v>
+      </c>
+      <c r="I31" s="101">
+        <v>45.973990999999998</v>
+      </c>
+      <c r="J31" s="101">
+        <v>48.728822999999998</v>
+      </c>
+      <c r="K31" s="101">
+        <v>45.953823999999997</v>
+      </c>
+      <c r="L31" s="101">
+        <v>43.102499000000002</v>
+      </c>
+      <c r="M31" s="101">
+        <v>33.083308000000002</v>
+      </c>
+      <c r="N31" s="101">
+        <v>35.434505999999999</v>
+      </c>
+      <c r="O31" s="101">
+        <v>41.122202000000001</v>
+      </c>
+      <c r="P31" s="101">
+        <v>41.020955999999998</v>
+      </c>
+      <c r="Q31" s="101">
+        <v>39.011172999999999</v>
+      </c>
+      <c r="R31" s="101">
+        <v>35.511139</v>
+      </c>
+      <c r="S31" s="101">
+        <v>28.93252</v>
+      </c>
+      <c r="T31" s="101">
+        <v>27.640864000000001</v>
+      </c>
+      <c r="U31" s="101">
+        <v>24.967200999999999</v>
+      </c>
+      <c r="V31" s="101">
+        <v>25.301928</v>
+      </c>
+    </row>
+    <row r="32" spans="2:22">
+      <c r="B32" s="109" t="s">
+        <v>210</v>
+      </c>
+      <c r="C32" s="101">
+        <v>19.393939</v>
+      </c>
+      <c r="D32" s="101">
+        <v>16.225418999999999</v>
+      </c>
+      <c r="E32" s="101">
+        <v>14.546766</v>
+      </c>
+      <c r="F32" s="101">
+        <v>9.5308010000000003</v>
+      </c>
+      <c r="G32" s="101">
+        <v>6.5328090000000003</v>
+      </c>
+      <c r="H32" s="101">
+        <v>6.6219200000000003</v>
+      </c>
+      <c r="I32" s="101">
+        <v>6.1692869999999997</v>
+      </c>
+      <c r="J32" s="101">
+        <v>5.7985569999999997</v>
+      </c>
+      <c r="K32" s="101">
+        <v>8.4910099999999993</v>
+      </c>
+      <c r="L32" s="101">
+        <v>6.7305549999999998</v>
+      </c>
+      <c r="M32" s="101">
+        <v>7.9295309999999999</v>
+      </c>
+      <c r="N32" s="101">
+        <v>9.1903349999999993</v>
+      </c>
+      <c r="O32" s="101">
+        <v>9.1728970000000007</v>
+      </c>
+      <c r="P32" s="101">
+        <v>7.4540569999999997</v>
+      </c>
+      <c r="Q32" s="101">
+        <v>9.1073939999999993</v>
+      </c>
+      <c r="R32" s="101">
+        <v>9.5381699999999991</v>
+      </c>
+      <c r="S32" s="101">
+        <v>12.234508</v>
+      </c>
+      <c r="T32" s="101">
+        <v>14.828619</v>
+      </c>
+      <c r="U32" s="101">
+        <v>13.290763</v>
+      </c>
+      <c r="V32" s="101">
+        <v>12.93585</v>
+      </c>
+    </row>
+    <row r="33" spans="1:22">
+      <c r="B33" s="107"/>
+    </row>
+    <row r="34" spans="1:22">
+      <c r="B34" s="99" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="35" spans="1:22">
+      <c r="B35" s="110" t="s">
+        <v>251</v>
+      </c>
+      <c r="C35" s="102">
+        <v>1548.5070000000001</v>
+      </c>
+      <c r="D35" s="102">
+        <v>1553.059</v>
+      </c>
+      <c r="E35" s="102">
+        <v>1596.9469999999999</v>
+      </c>
+      <c r="F35" s="102">
+        <v>1433.643</v>
+      </c>
+      <c r="G35" s="102">
+        <v>1420.8040000000001</v>
+      </c>
+      <c r="H35" s="102">
+        <v>1478.454</v>
+      </c>
+      <c r="I35" s="102">
+        <v>1450.481</v>
+      </c>
+      <c r="J35" s="102">
+        <v>1453.0050000000001</v>
+      </c>
+      <c r="K35" s="102">
+        <v>1574.2929999999999</v>
+      </c>
+      <c r="L35" s="102">
+        <v>1413.3520000000001</v>
+      </c>
+      <c r="M35" s="102">
+        <v>1403.8530000000001</v>
+      </c>
+      <c r="N35" s="102">
+        <v>1404.39</v>
+      </c>
+      <c r="O35" s="102">
+        <v>1373.8009999999999</v>
+      </c>
+      <c r="P35" s="102">
+        <v>1365.414</v>
+      </c>
+      <c r="Q35" s="102">
+        <v>1327.2170000000001</v>
+      </c>
+      <c r="R35" s="102">
+        <v>1349.3710000000001</v>
+      </c>
+      <c r="S35" s="102">
+        <v>1408.145</v>
+      </c>
+      <c r="T35" s="102">
+        <v>1528.6289999999999</v>
+      </c>
+      <c r="U35" s="102">
+        <v>1529.5309999999999</v>
+      </c>
+      <c r="V35" s="102">
+        <v>1739.2650000000001</v>
+      </c>
+    </row>
+    <row r="36" spans="1:22">
+      <c r="B36" s="110" t="s">
+        <v>193</v>
+      </c>
+      <c r="C36" s="102">
+        <v>322511</v>
+      </c>
+      <c r="D36" s="102">
+        <v>323211</v>
+      </c>
+      <c r="E36" s="102">
+        <v>317807</v>
+      </c>
+      <c r="F36" s="102">
+        <v>318263</v>
+      </c>
+      <c r="G36" s="102">
+        <v>338898</v>
+      </c>
+      <c r="H36" s="102">
+        <v>352140</v>
+      </c>
+      <c r="I36" s="102">
+        <v>352477</v>
+      </c>
+      <c r="J36" s="102">
+        <v>358832</v>
+      </c>
+      <c r="K36" s="102">
+        <v>340092</v>
+      </c>
+      <c r="L36" s="102">
+        <v>299829</v>
+      </c>
+      <c r="M36" s="102">
+        <v>341325</v>
+      </c>
+      <c r="N36" s="102">
+        <v>352091</v>
+      </c>
+      <c r="O36" s="102">
+        <v>371074</v>
+      </c>
+      <c r="P36" s="102">
+        <v>386132</v>
+      </c>
+      <c r="Q36" s="102">
+        <v>415462</v>
+      </c>
+      <c r="R36" s="102">
+        <v>411813</v>
+      </c>
+      <c r="S36" s="102">
+        <v>395889</v>
+      </c>
+      <c r="T36" s="102">
+        <v>423664</v>
+      </c>
+      <c r="U36" s="102">
+        <v>448319</v>
+      </c>
+      <c r="V36" s="102">
+        <v>451277</v>
+      </c>
+    </row>
+    <row r="37" spans="1:22">
+      <c r="B37" s="107"/>
+    </row>
+    <row r="38" spans="1:22" ht="26.25">
+      <c r="A38" s="15"/>
+      <c r="B38" s="99" t="s">
+        <v>323</v>
+      </c>
+      <c r="C38" s="74">
+        <v>1.920482</v>
+      </c>
+      <c r="D38" s="74">
+        <v>1.906296</v>
+      </c>
+      <c r="E38" s="74">
+        <v>1.722966</v>
+      </c>
+      <c r="F38" s="74">
+        <v>1.8189690000000001</v>
+      </c>
+      <c r="G38" s="74">
+        <v>1.7892429999999999</v>
+      </c>
+      <c r="H38" s="74">
+        <v>1.8056989999999999</v>
+      </c>
+      <c r="I38" s="74">
+        <v>1.8610139999999999</v>
+      </c>
+      <c r="J38" s="74">
+        <v>1.931551</v>
+      </c>
+      <c r="K38" s="74">
+        <v>2.004432</v>
+      </c>
+      <c r="L38" s="74">
+        <v>2.121022</v>
+      </c>
+      <c r="M38" s="74">
+        <v>1.762966</v>
+      </c>
+      <c r="N38" s="74">
+        <v>1.9699610000000001</v>
+      </c>
+      <c r="O38" s="74">
+        <v>1.7335309999999999</v>
+      </c>
+      <c r="P38" s="74">
+        <v>1.539866</v>
+      </c>
+      <c r="Q38" s="74">
+        <v>1.4979389999999999</v>
+      </c>
+      <c r="R38" s="74">
+        <v>1.4850749999999999</v>
+      </c>
+      <c r="S38" s="74">
+        <v>1.438202</v>
+      </c>
+      <c r="T38" s="74">
+        <v>1.4977879999999999</v>
+      </c>
+      <c r="U38" s="74">
+        <v>1.462726</v>
+      </c>
+      <c r="V38" s="74">
+        <v>1.3182579999999999</v>
+      </c>
+    </row>
+    <row r="39" spans="1:22" ht="26.25">
+      <c r="A39" s="15"/>
+      <c r="B39" s="99" t="s">
+        <v>324</v>
+      </c>
+      <c r="C39" s="74">
+        <v>0.252724</v>
+      </c>
+      <c r="D39" s="74">
+        <v>0.24981</v>
+      </c>
+      <c r="E39" s="74">
+        <v>0.23120499999999999</v>
+      </c>
+      <c r="F39" s="74">
+        <v>0.233622</v>
+      </c>
+      <c r="G39" s="74">
+        <v>0.226017</v>
+      </c>
+      <c r="H39" s="74">
+        <v>0.23188600000000001</v>
+      </c>
+      <c r="I39" s="74">
+        <v>0.242786</v>
+      </c>
+      <c r="J39" s="74">
+        <v>0.25569500000000001</v>
+      </c>
+      <c r="K39" s="74">
+        <v>0.28427400000000003</v>
+      </c>
+      <c r="L39" s="74">
+        <v>0.27468700000000001</v>
+      </c>
+      <c r="M39" s="74">
+        <v>0.238043</v>
+      </c>
+      <c r="N39" s="74">
+        <v>0.26014100000000001</v>
+      </c>
+      <c r="O39" s="74">
+        <v>0.25384800000000002</v>
+      </c>
+      <c r="P39" s="74">
+        <v>0.23553499999999999</v>
+      </c>
+      <c r="Q39" s="74">
+        <v>0.224853</v>
+      </c>
+      <c r="R39" s="74">
+        <v>0.21575800000000001</v>
+      </c>
+      <c r="S39" s="74">
+        <v>0.20574400000000001</v>
+      </c>
+      <c r="T39" s="74">
+        <v>0.220053</v>
+      </c>
+      <c r="U39" s="74">
+        <v>0.21263099999999999</v>
+      </c>
+      <c r="V39" s="74">
+        <v>0.21271200000000001</v>
+      </c>
+    </row>
+    <row r="40" spans="1:22">
+      <c r="B40" s="107"/>
+    </row>
+    <row r="41" spans="1:22">
+      <c r="B41" s="107"/>
+    </row>
+    <row r="42" spans="1:22" ht="28.5">
+      <c r="A42" s="15"/>
+      <c r="B42" s="103" t="s">
+        <v>325</v>
+      </c>
+      <c r="C42" s="65">
+        <v>6.5970870000000001</v>
+      </c>
+      <c r="D42" s="65">
+        <v>6.5363329999999999</v>
+      </c>
+      <c r="E42" s="65">
+        <v>5.9528410000000003</v>
+      </c>
+      <c r="F42" s="65">
+        <v>6.009925</v>
+      </c>
+      <c r="G42" s="65">
+        <v>6.1800059999999997</v>
+      </c>
+      <c r="H42" s="65">
+        <v>6.5850609999999996</v>
+      </c>
+      <c r="I42" s="65">
+        <v>6.8935190000000004</v>
+      </c>
+      <c r="J42" s="65">
+        <v>7.3840839999999996</v>
+      </c>
+      <c r="K42" s="65">
+        <v>7.7961669999999996</v>
+      </c>
+      <c r="L42" s="65">
+        <v>6.6655730000000002</v>
+      </c>
+      <c r="M42" s="65">
+        <v>6.5381289999999996</v>
+      </c>
+      <c r="N42" s="65">
+        <v>7.3686220000000002</v>
+      </c>
+      <c r="O42" s="65">
+        <v>7.5418260000000004</v>
+      </c>
+      <c r="P42" s="65">
+        <v>7.2663229999999999</v>
+      </c>
+      <c r="Q42" s="65">
+        <v>7.450304</v>
+      </c>
+      <c r="R42" s="65">
+        <v>7.0949920000000004</v>
+      </c>
+      <c r="S42" s="65">
+        <v>6.5187629999999999</v>
+      </c>
+      <c r="T42" s="65">
+        <v>7.4590500000000004</v>
+      </c>
+      <c r="U42" s="65">
+        <v>7.618824</v>
+      </c>
+      <c r="V42" s="65">
+        <v>7.6751269999999998</v>
+      </c>
+    </row>
+    <row r="43" spans="1:22">
+      <c r="A43" s="15"/>
+      <c r="B43" s="107" t="s">
+        <v>321</v>
+      </c>
+      <c r="C43" s="104">
+        <v>0.23223199999999999</v>
+      </c>
+      <c r="D43" s="104">
+        <v>0.23119400000000001</v>
+      </c>
+      <c r="E43" s="104">
+        <v>0.214865</v>
+      </c>
+      <c r="F43" s="104">
+        <v>0.20364099999999999</v>
+      </c>
+      <c r="G43" s="104">
+        <v>0.198519</v>
+      </c>
+      <c r="H43" s="104">
+        <v>0.20847399999999999</v>
+      </c>
+      <c r="I43" s="104">
+        <v>0.21079500000000001</v>
+      </c>
+      <c r="J43" s="104">
+        <v>0.219165</v>
+      </c>
+      <c r="K43" s="104">
+        <v>0.24642</v>
+      </c>
+      <c r="L43" s="104">
+        <v>0.234096</v>
+      </c>
+      <c r="M43" s="104">
+        <v>0.19327</v>
+      </c>
+      <c r="N43" s="104">
+        <v>0.21604499999999999</v>
+      </c>
+      <c r="O43" s="104">
+        <v>0.185975</v>
+      </c>
+      <c r="P43" s="104">
+        <v>0.16419</v>
+      </c>
+      <c r="Q43" s="104">
+        <v>0.155251</v>
+      </c>
+      <c r="R43" s="104">
+        <v>0.15648699999999999</v>
+      </c>
+      <c r="S43" s="104">
+        <v>0.15814900000000001</v>
+      </c>
+      <c r="T43" s="104">
+        <v>0.17879300000000001</v>
+      </c>
+      <c r="U43" s="104">
+        <v>0.17471100000000001</v>
+      </c>
+      <c r="V43" s="104">
+        <v>0.17904600000000001</v>
+      </c>
+    </row>
+    <row r="44" spans="1:22">
+      <c r="A44" s="15"/>
+      <c r="B44" s="107" t="s">
+        <v>322</v>
+      </c>
+      <c r="C44" s="104">
+        <v>6.3648559999999996</v>
+      </c>
+      <c r="D44" s="104">
+        <v>6.3051389999999996</v>
+      </c>
+      <c r="E44" s="104">
+        <v>5.7379759999999997</v>
+      </c>
+      <c r="F44" s="104">
+        <v>5.8062839999999998</v>
+      </c>
+      <c r="G44" s="104">
+        <v>5.9814870000000004</v>
+      </c>
+      <c r="H44" s="104">
+        <v>6.3765879999999999</v>
+      </c>
+      <c r="I44" s="104">
+        <v>6.6827240000000003</v>
+      </c>
+      <c r="J44" s="104">
+        <v>7.1649180000000001</v>
+      </c>
+      <c r="K44" s="104">
+        <v>7.5497480000000001</v>
+      </c>
+      <c r="L44" s="104">
+        <v>6.4314770000000001</v>
+      </c>
+      <c r="M44" s="104">
+        <v>6.3448589999999996</v>
+      </c>
+      <c r="N44" s="104">
+        <v>7.152577</v>
+      </c>
+      <c r="O44" s="104">
+        <v>7.3558519999999996</v>
+      </c>
+      <c r="P44" s="104">
+        <v>7.1021340000000004</v>
+      </c>
+      <c r="Q44" s="104">
+        <v>7.2950530000000002</v>
+      </c>
+      <c r="R44" s="104">
+        <v>6.9385060000000003</v>
+      </c>
+      <c r="S44" s="104">
+        <v>6.360614</v>
+      </c>
+      <c r="T44" s="104">
+        <v>7.2802569999999998</v>
+      </c>
+      <c r="U44" s="104">
+        <v>7.4441129999999998</v>
+      </c>
+      <c r="V44" s="104">
+        <v>7.4960810000000002</v>
+      </c>
+    </row>
+    <row r="45" spans="1:22">
+      <c r="B45" s="108" t="s">
+        <v>212</v>
+      </c>
+      <c r="C45" s="101"/>
+      <c r="D45" s="101"/>
+      <c r="E45" s="101"/>
+      <c r="F45" s="101"/>
+      <c r="G45" s="101"/>
+      <c r="H45" s="101"/>
+      <c r="I45" s="101"/>
+      <c r="J45" s="101"/>
+      <c r="K45" s="101"/>
+      <c r="L45" s="101"/>
+      <c r="M45" s="101"/>
+      <c r="N45" s="101"/>
+      <c r="O45" s="101"/>
+      <c r="P45" s="101"/>
+      <c r="Q45" s="101"/>
+      <c r="R45" s="101"/>
+      <c r="S45" s="101"/>
+      <c r="T45" s="101"/>
+      <c r="U45" s="101"/>
+      <c r="V45" s="101"/>
+    </row>
+    <row r="46" spans="1:22">
+      <c r="B46" s="107" t="s">
+        <v>201</v>
+      </c>
+      <c r="C46" s="101">
+        <v>0</v>
+      </c>
+      <c r="D46" s="101">
+        <v>0</v>
+      </c>
+      <c r="E46" s="101">
+        <v>0</v>
+      </c>
+      <c r="F46" s="101">
+        <v>0</v>
+      </c>
+      <c r="G46" s="101">
+        <v>0</v>
+      </c>
+      <c r="H46" s="101">
+        <v>0</v>
+      </c>
+      <c r="I46" s="101">
+        <v>0</v>
+      </c>
+      <c r="J46" s="101">
+        <v>0</v>
+      </c>
+      <c r="K46" s="101">
+        <v>0</v>
+      </c>
+      <c r="L46" s="101">
+        <v>0</v>
+      </c>
+      <c r="M46" s="101">
+        <v>0</v>
+      </c>
+      <c r="N46" s="101">
+        <v>0</v>
+      </c>
+      <c r="O46" s="101">
+        <v>0</v>
+      </c>
+      <c r="P46" s="101">
+        <v>0</v>
+      </c>
+      <c r="Q46" s="101">
+        <v>0</v>
+      </c>
+      <c r="R46" s="101">
+        <v>0</v>
+      </c>
+      <c r="S46" s="101">
+        <v>0</v>
+      </c>
+      <c r="T46" s="101">
+        <v>0</v>
+      </c>
+      <c r="U46" s="101">
+        <v>0</v>
+      </c>
+      <c r="V46" s="101">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="47" spans="1:22">
+      <c r="B47" s="107" t="s">
+        <v>202</v>
+      </c>
+      <c r="C47" s="101">
+        <v>0</v>
+      </c>
+      <c r="D47" s="101">
+        <v>0</v>
+      </c>
+      <c r="E47" s="101">
+        <v>0</v>
+      </c>
+      <c r="F47" s="101">
+        <v>0</v>
+      </c>
+      <c r="G47" s="101">
+        <v>0</v>
+      </c>
+      <c r="H47" s="101">
+        <v>0</v>
+      </c>
+      <c r="I47" s="101">
+        <v>0</v>
+      </c>
+      <c r="J47" s="101">
+        <v>0</v>
+      </c>
+      <c r="K47" s="101">
+        <v>0</v>
+      </c>
+      <c r="L47" s="101">
+        <v>0</v>
+      </c>
+      <c r="M47" s="101">
+        <v>0</v>
+      </c>
+      <c r="N47" s="101">
+        <v>0</v>
+      </c>
+      <c r="O47" s="101">
+        <v>0</v>
+      </c>
+      <c r="P47" s="101">
+        <v>0</v>
+      </c>
+      <c r="Q47" s="101">
+        <v>0</v>
+      </c>
+      <c r="R47" s="101">
+        <v>0</v>
+      </c>
+      <c r="S47" s="101">
+        <v>0</v>
+      </c>
+      <c r="T47" s="101">
+        <v>0</v>
+      </c>
+      <c r="U47" s="101">
+        <v>0</v>
+      </c>
+      <c r="V47" s="101">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="48" spans="1:22">
+      <c r="B48" s="107" t="s">
+        <v>203</v>
+      </c>
+      <c r="C48" s="101">
+        <v>7.3638999999999996E-2</v>
+      </c>
+      <c r="D48" s="101">
+        <v>6.9110000000000005E-2</v>
+      </c>
+      <c r="E48" s="101">
+        <v>7.7310000000000004E-2</v>
+      </c>
+      <c r="F48" s="101">
+        <v>0.16461500000000001</v>
+      </c>
+      <c r="G48" s="101">
+        <v>0.11752600000000001</v>
+      </c>
+      <c r="H48" s="101">
+        <v>0.11479300000000001</v>
+      </c>
+      <c r="I48" s="101">
+        <v>0.10432900000000001</v>
+      </c>
+      <c r="J48" s="101">
+        <v>0.15485399999999999</v>
+      </c>
+      <c r="K48" s="101">
+        <v>0.13868900000000001</v>
+      </c>
+      <c r="L48" s="101">
+        <v>0.11518399999999999</v>
+      </c>
+      <c r="M48" s="101">
+        <v>0.13650200000000001</v>
+      </c>
+      <c r="N48" s="101">
+        <v>0.169847</v>
+      </c>
+      <c r="O48" s="101">
+        <v>0.13088</v>
+      </c>
+      <c r="P48" s="101">
+        <v>0.104407</v>
+      </c>
+      <c r="Q48" s="101">
+        <v>0.108233</v>
+      </c>
+      <c r="R48" s="101">
+        <v>0.117995</v>
+      </c>
+      <c r="S48" s="101">
+        <v>0.119244</v>
+      </c>
+      <c r="T48" s="101">
+        <v>0.151339</v>
+      </c>
+      <c r="U48" s="101">
+        <v>0.162663</v>
+      </c>
+      <c r="V48" s="101">
+        <v>0.15836800000000001</v>
+      </c>
+    </row>
+    <row r="49" spans="2:22">
+      <c r="B49" s="107" t="s">
+        <v>204</v>
+      </c>
+      <c r="C49" s="101">
+        <v>0.233178</v>
+      </c>
+      <c r="D49" s="101">
+        <v>0.259573</v>
+      </c>
+      <c r="E49" s="101">
+        <v>0.25840200000000002</v>
+      </c>
+      <c r="F49" s="101">
+        <v>0.28112599999999999</v>
+      </c>
+      <c r="G49" s="101">
+        <v>0.29120000000000001</v>
+      </c>
+      <c r="H49" s="101">
+        <v>0.28448400000000001</v>
+      </c>
+      <c r="I49" s="101">
+        <v>0.28276600000000002</v>
+      </c>
+      <c r="J49" s="101">
+        <v>0.28573300000000001</v>
+      </c>
+      <c r="K49" s="101">
+        <v>0.245673</v>
+      </c>
+      <c r="L49" s="101">
+        <v>0.252467</v>
+      </c>
+      <c r="M49" s="101">
+        <v>0.306037</v>
+      </c>
+      <c r="N49" s="101">
+        <v>0.28948200000000002</v>
+      </c>
+      <c r="O49" s="101">
+        <v>0.27284799999999998</v>
+      </c>
+      <c r="P49" s="101">
+        <v>0.197881</v>
+      </c>
+      <c r="Q49" s="101">
+        <v>0.204129</v>
+      </c>
+      <c r="R49" s="101">
+        <v>0.17133100000000001</v>
+      </c>
+      <c r="S49" s="101">
+        <v>0.159695</v>
+      </c>
+      <c r="T49" s="101">
+        <v>0.157196</v>
+      </c>
+      <c r="U49" s="101">
+        <v>0.15961700000000001</v>
+      </c>
+      <c r="V49" s="101">
+        <v>0.15063699999999999</v>
+      </c>
+    </row>
+    <row r="50" spans="2:22">
+      <c r="B50" s="109" t="s">
+        <v>205</v>
+      </c>
+      <c r="C50" s="101">
+        <v>0.80566000000000004</v>
+      </c>
+      <c r="D50" s="101">
+        <v>0.75693100000000002</v>
+      </c>
+      <c r="E50" s="101">
+        <v>0.74615500000000001</v>
+      </c>
+      <c r="F50" s="101">
+        <v>0.741313</v>
+      </c>
+      <c r="G50" s="101">
+        <v>0.81159499999999996</v>
+      </c>
+      <c r="H50" s="101">
+        <v>0.70547000000000004</v>
+      </c>
+      <c r="I50" s="101">
+        <v>0.76653700000000002</v>
+      </c>
+      <c r="J50" s="101">
+        <v>0.88109499999999996</v>
+      </c>
+      <c r="K50" s="101">
+        <v>0.88890400000000003</v>
+      </c>
+      <c r="L50" s="101">
+        <v>0.92505999999999999</v>
+      </c>
+      <c r="M50" s="101">
+        <v>0.84369000000000005</v>
+      </c>
+      <c r="N50" s="101">
+        <v>0.88945099999999999</v>
+      </c>
+      <c r="O50" s="101">
+        <v>0.92857400000000001</v>
+      </c>
+      <c r="P50" s="101">
+        <v>0.86680500000000005</v>
+      </c>
+      <c r="Q50" s="101">
+        <v>0.77411099999999999</v>
+      </c>
+      <c r="R50" s="101">
+        <v>0.67985600000000002</v>
+      </c>
+      <c r="S50" s="101">
+        <v>0.67118800000000001</v>
+      </c>
+      <c r="T50" s="101">
+        <v>0.619336</v>
+      </c>
+      <c r="U50" s="101">
+        <v>0.69406900000000005</v>
+      </c>
+      <c r="V50" s="101">
+        <v>0.63667200000000002</v>
+      </c>
+    </row>
+    <row r="51" spans="2:22">
+      <c r="B51" s="109" t="s">
+        <v>206</v>
+      </c>
+      <c r="C51" s="101">
+        <v>1.6696530000000001</v>
+      </c>
+      <c r="D51" s="101">
+        <v>1.580084</v>
+      </c>
+      <c r="E51" s="101">
+        <v>1.460917</v>
+      </c>
+      <c r="F51" s="101">
+        <v>1.2817000000000001</v>
+      </c>
+      <c r="G51" s="101">
+        <v>1.4457679999999999</v>
+      </c>
+      <c r="H51" s="101">
+        <v>1.5522830000000001</v>
+      </c>
+      <c r="I51" s="101">
+        <v>1.472475</v>
+      </c>
+      <c r="J51" s="101">
+        <v>1.533776</v>
+      </c>
+      <c r="K51" s="101">
+        <v>1.5319799999999999</v>
+      </c>
+      <c r="L51" s="101">
+        <v>1.1497269999999999</v>
+      </c>
+      <c r="M51" s="101">
+        <v>1.253665</v>
+      </c>
+      <c r="N51" s="101">
+        <v>1.3213699999999999</v>
+      </c>
+      <c r="O51" s="101">
+        <v>1.239687</v>
+      </c>
+      <c r="P51" s="101">
+        <v>1.313483</v>
+      </c>
+      <c r="Q51" s="101">
+        <v>1.4093</v>
+      </c>
+      <c r="R51" s="101">
+        <v>1.427573</v>
+      </c>
+      <c r="S51" s="101">
+        <v>1.44733</v>
+      </c>
+      <c r="T51" s="101">
+        <v>1.4411609999999999</v>
+      </c>
+      <c r="U51" s="101">
+        <v>1.5318240000000001</v>
+      </c>
+      <c r="V51" s="101">
+        <v>1.549863</v>
+      </c>
+    </row>
+    <row r="52" spans="2:22">
+      <c r="B52" s="109" t="s">
+        <v>207</v>
+      </c>
+      <c r="C52" s="101">
+        <v>0.320718</v>
+      </c>
+      <c r="D52" s="101">
+        <v>0.243564</v>
+      </c>
+      <c r="E52" s="101">
+        <v>9.0351000000000001E-2</v>
+      </c>
+      <c r="F52" s="101">
+        <v>0.202567</v>
+      </c>
+      <c r="G52" s="101">
+        <v>0.293464</v>
+      </c>
+      <c r="H52" s="101">
+        <v>0.298931</v>
+      </c>
+      <c r="I52" s="101">
+        <v>0.292215</v>
+      </c>
+      <c r="J52" s="101">
+        <v>0.25379400000000002</v>
+      </c>
+      <c r="K52" s="101">
+        <v>0.27495700000000001</v>
+      </c>
+      <c r="L52" s="101">
+        <v>0.52250399999999997</v>
+      </c>
+      <c r="M52" s="101">
+        <v>0.62378699999999998</v>
+      </c>
+      <c r="N52" s="101">
+        <v>0.69032000000000004</v>
+      </c>
+      <c r="O52" s="101">
+        <v>0.61558800000000002</v>
+      </c>
+      <c r="P52" s="101">
+        <v>0.56826500000000002</v>
+      </c>
+      <c r="Q52" s="101">
+        <v>0.65369600000000005</v>
+      </c>
+      <c r="R52" s="101">
+        <v>0.702268</v>
+      </c>
+      <c r="S52" s="101">
+        <v>0.65853700000000004</v>
+      </c>
+      <c r="T52" s="101">
+        <v>0.80089600000000005</v>
+      </c>
+      <c r="U52" s="101">
+        <v>0.87836199999999998</v>
+      </c>
+      <c r="V52" s="101">
+        <v>0.89062200000000002</v>
+      </c>
+    </row>
+    <row r="53" spans="2:22">
+      <c r="B53" s="109" t="s">
+        <v>208</v>
+      </c>
+      <c r="C53" s="101">
+        <v>0.40903800000000001</v>
+      </c>
+      <c r="D53" s="101">
+        <v>0.30353799999999997</v>
+      </c>
+      <c r="E53" s="101">
+        <v>0.245282</v>
+      </c>
+      <c r="F53" s="101">
+        <v>0.18835399999999999</v>
+      </c>
+      <c r="G53" s="101">
+        <v>0.169847</v>
+      </c>
+      <c r="H53" s="101">
+        <v>0.41021000000000002</v>
+      </c>
+      <c r="I53" s="101">
+        <v>0.380691</v>
+      </c>
+      <c r="J53" s="101">
+        <v>0.24848400000000001</v>
+      </c>
+      <c r="K53" s="101">
+        <v>0.471354</v>
+      </c>
+      <c r="L53" s="101">
+        <v>0.378973</v>
+      </c>
+      <c r="M53" s="101">
+        <v>0.69297500000000001</v>
+      </c>
+      <c r="N53" s="101">
+        <v>0.71991700000000003</v>
+      </c>
+      <c r="O53" s="101">
+        <v>0.56108000000000002</v>
+      </c>
+      <c r="P53" s="101">
+        <v>0.69313100000000005</v>
+      </c>
+      <c r="Q53" s="101">
+        <v>0.71585600000000005</v>
+      </c>
+      <c r="R53" s="101">
+        <v>0.79972500000000002</v>
+      </c>
+      <c r="S53" s="101">
+        <v>0.77918699999999996</v>
+      </c>
+      <c r="T53" s="101">
+        <v>1.121302</v>
+      </c>
+      <c r="U53" s="101">
+        <v>1.2774829999999999</v>
+      </c>
+      <c r="V53" s="101">
+        <v>1.354168</v>
+      </c>
+    </row>
+    <row r="54" spans="2:22">
+      <c r="B54" s="109" t="s">
+        <v>209</v>
+      </c>
+      <c r="C54" s="101">
+        <v>1.8057650000000001</v>
+      </c>
+      <c r="D54" s="101">
+        <v>2.262985</v>
+      </c>
+      <c r="E54" s="101">
+        <v>2.2084779999999999</v>
+      </c>
+      <c r="F54" s="101">
+        <v>2.5774560000000002</v>
+      </c>
+      <c r="G54" s="101">
+        <v>2.6468780000000001</v>
+      </c>
+      <c r="H54" s="101">
+        <v>2.7828339999999998</v>
+      </c>
+      <c r="I54" s="101">
+        <v>3.1692260000000001</v>
+      </c>
+      <c r="J54" s="101">
+        <v>3.5981770000000002</v>
+      </c>
+      <c r="K54" s="101">
+        <v>3.5826370000000001</v>
+      </c>
+      <c r="L54" s="101">
+        <v>2.8730280000000001</v>
+      </c>
+      <c r="M54" s="101">
+        <v>2.1630289999999999</v>
+      </c>
+      <c r="N54" s="101">
+        <v>2.6110350000000002</v>
+      </c>
+      <c r="O54" s="101">
+        <v>3.1013649999999999</v>
+      </c>
+      <c r="P54" s="101">
+        <v>2.980715</v>
+      </c>
+      <c r="Q54" s="101">
+        <v>2.9064510000000001</v>
+      </c>
+      <c r="R54" s="101">
+        <v>2.5195129999999999</v>
+      </c>
+      <c r="S54" s="101">
+        <v>1.886042</v>
+      </c>
+      <c r="T54" s="101">
+        <v>2.0617459999999999</v>
+      </c>
+      <c r="U54" s="101">
+        <v>1.902207</v>
+      </c>
+      <c r="V54" s="101">
+        <v>1.9419550000000001</v>
+      </c>
+    </row>
+    <row r="55" spans="2:22">
+      <c r="B55" s="109" t="s">
+        <v>210</v>
+      </c>
+      <c r="C55" s="101">
+        <v>1.2794350000000001</v>
+      </c>
+      <c r="D55" s="101">
+        <v>1.0605469999999999</v>
+      </c>
+      <c r="E55" s="101">
+        <v>0.86594599999999999</v>
+      </c>
+      <c r="F55" s="101">
+        <v>0.57279400000000003</v>
+      </c>
+      <c r="G55" s="101">
+        <v>0.40372799999999998</v>
+      </c>
+      <c r="H55" s="101">
+        <v>0.43605699999999997</v>
+      </c>
+      <c r="I55" s="101">
+        <v>0.42528100000000002</v>
+      </c>
+      <c r="J55" s="101">
+        <v>0.42817</v>
+      </c>
+      <c r="K55" s="101">
+        <v>0.66197300000000003</v>
+      </c>
+      <c r="L55" s="101">
+        <v>0.44862999999999997</v>
+      </c>
+      <c r="M55" s="101">
+        <v>0.51844299999999999</v>
+      </c>
+      <c r="N55" s="101">
+        <v>0.67720100000000005</v>
+      </c>
+      <c r="O55" s="101">
+        <v>0.69180399999999997</v>
+      </c>
+      <c r="P55" s="101">
+        <v>0.54163600000000001</v>
+      </c>
+      <c r="Q55" s="101">
+        <v>0.67852900000000005</v>
+      </c>
+      <c r="R55" s="101">
+        <v>0.676732</v>
+      </c>
+      <c r="S55" s="101">
+        <v>0.797539</v>
+      </c>
+      <c r="T55" s="101">
+        <v>1.106074</v>
+      </c>
+      <c r="U55" s="101">
+        <v>1.0125999999999999</v>
+      </c>
+      <c r="V55" s="101">
+        <v>0.99284300000000003</v>
+      </c>
+    </row>
+    <row r="56" spans="2:22">
+      <c r="B56" s="107"/>
+      <c r="C56" s="101"/>
+      <c r="D56" s="101"/>
+      <c r="E56" s="101"/>
+      <c r="F56" s="101"/>
+      <c r="G56" s="101"/>
+      <c r="H56" s="101"/>
+      <c r="I56" s="101"/>
+      <c r="J56" s="101"/>
+      <c r="K56" s="101"/>
+      <c r="L56" s="101"/>
+      <c r="M56" s="101"/>
+      <c r="N56" s="101"/>
+      <c r="O56" s="101"/>
+      <c r="P56" s="101"/>
+      <c r="Q56" s="101"/>
+      <c r="R56" s="101"/>
+      <c r="S56" s="101"/>
+      <c r="T56" s="101"/>
+      <c r="U56" s="101"/>
+      <c r="V56" s="101"/>
+    </row>
+    <row r="57" spans="2:22">
+      <c r="B57" s="108" t="s">
+        <v>192</v>
+      </c>
+      <c r="C57" s="101"/>
+      <c r="D57" s="101"/>
+      <c r="E57" s="101"/>
+      <c r="F57" s="101"/>
+      <c r="G57" s="101"/>
+      <c r="H57" s="101"/>
+      <c r="I57" s="101"/>
+      <c r="J57" s="101"/>
+      <c r="K57" s="101"/>
+      <c r="L57" s="101"/>
+      <c r="M57" s="101"/>
+      <c r="N57" s="101"/>
+      <c r="O57" s="101"/>
+      <c r="P57" s="101"/>
+      <c r="Q57" s="101"/>
+      <c r="R57" s="101"/>
+      <c r="S57" s="101"/>
+      <c r="T57" s="101"/>
+      <c r="U57" s="101"/>
+      <c r="V57" s="101"/>
+    </row>
+    <row r="58" spans="2:22">
+      <c r="B58" s="107" t="s">
+        <v>201</v>
+      </c>
+      <c r="C58" s="101">
+        <v>0</v>
+      </c>
+      <c r="D58" s="101">
+        <v>0</v>
+      </c>
+      <c r="E58" s="101">
+        <v>0</v>
+      </c>
+      <c r="F58" s="101">
+        <v>0</v>
+      </c>
+      <c r="G58" s="101">
+        <v>0</v>
+      </c>
+      <c r="H58" s="101">
+        <v>0</v>
+      </c>
+      <c r="I58" s="101">
+        <v>0</v>
+      </c>
+      <c r="J58" s="101">
+        <v>0</v>
+      </c>
+      <c r="K58" s="101">
+        <v>0</v>
+      </c>
+      <c r="L58" s="101">
+        <v>0</v>
+      </c>
+      <c r="M58" s="101">
+        <v>0</v>
+      </c>
+      <c r="N58" s="101">
+        <v>0</v>
+      </c>
+      <c r="O58" s="101">
+        <v>0</v>
+      </c>
+      <c r="P58" s="101">
+        <v>0</v>
+      </c>
+      <c r="Q58" s="101">
+        <v>0</v>
+      </c>
+      <c r="R58" s="101">
+        <v>0</v>
+      </c>
+      <c r="S58" s="101">
+        <v>0</v>
+      </c>
+      <c r="T58" s="101">
+        <v>0</v>
+      </c>
+      <c r="U58" s="101">
+        <v>0</v>
+      </c>
+      <c r="V58" s="101">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="59" spans="2:22">
+      <c r="B59" s="107" t="s">
+        <v>202</v>
+      </c>
+      <c r="C59" s="101">
+        <v>0</v>
+      </c>
+      <c r="D59" s="101">
+        <v>0</v>
+      </c>
+      <c r="E59" s="101">
+        <v>0</v>
+      </c>
+      <c r="F59" s="101">
+        <v>0</v>
+      </c>
+      <c r="G59" s="101">
+        <v>0</v>
+      </c>
+      <c r="H59" s="101">
+        <v>0</v>
+      </c>
+      <c r="I59" s="101">
+        <v>0</v>
+      </c>
+      <c r="J59" s="101">
+        <v>0</v>
+      </c>
+      <c r="K59" s="101">
+        <v>0</v>
+      </c>
+      <c r="L59" s="101">
+        <v>0</v>
+      </c>
+      <c r="M59" s="101">
+        <v>0</v>
+      </c>
+      <c r="N59" s="101">
+        <v>0</v>
+      </c>
+      <c r="O59" s="101">
+        <v>0</v>
+      </c>
+      <c r="P59" s="101">
+        <v>0</v>
+      </c>
+      <c r="Q59" s="101">
+        <v>0</v>
+      </c>
+      <c r="R59" s="101">
+        <v>0</v>
+      </c>
+      <c r="S59" s="101">
+        <v>0</v>
+      </c>
+      <c r="T59" s="101">
+        <v>0</v>
+      </c>
+      <c r="U59" s="101">
+        <v>0</v>
+      </c>
+      <c r="V59" s="101">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="60" spans="2:22">
+      <c r="B60" s="107" t="s">
+        <v>203</v>
+      </c>
+      <c r="C60" s="101">
+        <v>1.116241</v>
+      </c>
+      <c r="D60" s="101">
+        <v>1.0573220000000001</v>
+      </c>
+      <c r="E60" s="101">
+        <v>1.2987010000000001</v>
+      </c>
+      <c r="F60" s="101">
+        <v>2.7390500000000002</v>
+      </c>
+      <c r="G60" s="101">
+        <v>1.9017170000000001</v>
+      </c>
+      <c r="H60" s="101">
+        <v>1.7432350000000001</v>
+      </c>
+      <c r="I60" s="101">
+        <v>1.5134350000000001</v>
+      </c>
+      <c r="J60" s="101">
+        <v>2.0971259999999998</v>
+      </c>
+      <c r="K60" s="101">
+        <v>1.7789349999999999</v>
+      </c>
+      <c r="L60" s="101">
+        <v>1.7280359999999999</v>
+      </c>
+      <c r="M60" s="101">
+        <v>2.0877870000000001</v>
+      </c>
+      <c r="N60" s="101">
+        <v>2.305002</v>
+      </c>
+      <c r="O60" s="101">
+        <v>1.735385</v>
+      </c>
+      <c r="P60" s="101">
+        <v>1.4368620000000001</v>
+      </c>
+      <c r="Q60" s="101">
+        <v>1.452739</v>
+      </c>
+      <c r="R60" s="101">
+        <v>1.663071</v>
+      </c>
+      <c r="S60" s="101">
+        <v>1.8292459999999999</v>
+      </c>
+      <c r="T60" s="101">
+        <v>2.028937</v>
+      </c>
+      <c r="U60" s="101">
+        <v>2.1350090000000002</v>
+      </c>
+      <c r="V60" s="101">
+        <v>2.0633870000000001</v>
+      </c>
+    </row>
+    <row r="61" spans="2:22">
+      <c r="B61" s="107" t="s">
+        <v>204</v>
+      </c>
+      <c r="C61" s="101">
+        <v>3.534564</v>
+      </c>
+      <c r="D61" s="101">
+        <v>3.971231</v>
+      </c>
+      <c r="E61" s="101">
+        <v>4.3408110000000004</v>
+      </c>
+      <c r="F61" s="101">
+        <v>4.6776939999999998</v>
+      </c>
+      <c r="G61" s="101">
+        <v>4.7119619999999998</v>
+      </c>
+      <c r="H61" s="101">
+        <v>4.3201390000000002</v>
+      </c>
+      <c r="I61" s="101">
+        <v>4.1019079999999999</v>
+      </c>
+      <c r="J61" s="101">
+        <v>3.869583</v>
+      </c>
+      <c r="K61" s="101">
+        <v>3.1511990000000001</v>
+      </c>
+      <c r="L61" s="101">
+        <v>3.7876210000000001</v>
+      </c>
+      <c r="M61" s="101">
+        <v>4.6807999999999996</v>
+      </c>
+      <c r="N61" s="101">
+        <v>3.9285709999999998</v>
+      </c>
+      <c r="O61" s="101">
+        <v>3.617801</v>
+      </c>
+      <c r="P61" s="101">
+        <v>2.7232669999999999</v>
+      </c>
+      <c r="Q61" s="101">
+        <v>2.7398699999999998</v>
+      </c>
+      <c r="R61" s="101">
+        <v>2.4148100000000001</v>
+      </c>
+      <c r="S61" s="101">
+        <v>2.4497770000000001</v>
+      </c>
+      <c r="T61" s="101">
+        <v>2.107456</v>
+      </c>
+      <c r="U61" s="101">
+        <v>2.0950350000000002</v>
+      </c>
+      <c r="V61" s="101">
+        <v>1.9626600000000001</v>
+      </c>
+    </row>
+    <row r="62" spans="2:22">
+      <c r="B62" s="109" t="s">
+        <v>205</v>
+      </c>
+      <c r="C62" s="101">
+        <v>12.212358</v>
+      </c>
+      <c r="D62" s="101">
+        <v>11.580368</v>
+      </c>
+      <c r="E62" s="101">
+        <v>12.534435</v>
+      </c>
+      <c r="F62" s="101">
+        <v>12.334819</v>
+      </c>
+      <c r="G62" s="101">
+        <v>13.132588999999999</v>
+      </c>
+      <c r="H62" s="101">
+        <v>10.713184999999999</v>
+      </c>
+      <c r="I62" s="101">
+        <v>11.119669999999999</v>
+      </c>
+      <c r="J62" s="101">
+        <v>11.932359</v>
+      </c>
+      <c r="K62" s="101">
+        <v>11.401813000000001</v>
+      </c>
+      <c r="L62" s="101">
+        <v>13.878182000000001</v>
+      </c>
+      <c r="M62" s="101">
+        <v>12.90415</v>
+      </c>
+      <c r="N62" s="101">
+        <v>12.070793</v>
+      </c>
+      <c r="O62" s="101">
+        <v>12.312328000000001</v>
+      </c>
+      <c r="P62" s="101">
+        <v>11.929069999999999</v>
+      </c>
+      <c r="Q62" s="101">
+        <v>10.390332000000001</v>
+      </c>
+      <c r="R62" s="101">
+        <v>9.5821959999999997</v>
+      </c>
+      <c r="S62" s="101">
+        <v>10.296249</v>
+      </c>
+      <c r="T62" s="101">
+        <v>8.3031469999999992</v>
+      </c>
+      <c r="U62" s="101">
+        <v>9.1099180000000004</v>
+      </c>
+      <c r="V62" s="101">
+        <v>8.2952639999999995</v>
+      </c>
+    </row>
+    <row r="63" spans="2:22">
+      <c r="B63" s="109" t="s">
+        <v>206</v>
+      </c>
+      <c r="C63" s="101">
+        <v>25.308948999999998</v>
+      </c>
+      <c r="D63" s="101">
+        <v>24.173855</v>
+      </c>
+      <c r="E63" s="101">
+        <v>24.541519000000001</v>
+      </c>
+      <c r="F63" s="101">
+        <v>21.326385999999999</v>
+      </c>
+      <c r="G63" s="101">
+        <v>23.394280999999999</v>
+      </c>
+      <c r="H63" s="101">
+        <v>23.572800999999998</v>
+      </c>
+      <c r="I63" s="101">
+        <v>21.360278999999998</v>
+      </c>
+      <c r="J63" s="101">
+        <v>20.771377999999999</v>
+      </c>
+      <c r="K63" s="101">
+        <v>19.650423</v>
+      </c>
+      <c r="L63" s="101">
+        <v>17.248732</v>
+      </c>
+      <c r="M63" s="101">
+        <v>19.174679000000001</v>
+      </c>
+      <c r="N63" s="101">
+        <v>17.932386999999999</v>
+      </c>
+      <c r="O63" s="101">
+        <v>16.437491000000001</v>
+      </c>
+      <c r="P63" s="101">
+        <v>18.076302999999999</v>
+      </c>
+      <c r="Q63" s="101">
+        <v>18.916001000000001</v>
+      </c>
+      <c r="R63" s="101">
+        <v>20.120850999999998</v>
+      </c>
+      <c r="S63" s="101">
+        <v>22.202522999999999</v>
+      </c>
+      <c r="T63" s="101">
+        <v>19.320965999999999</v>
+      </c>
+      <c r="U63" s="101">
+        <v>20.105777</v>
+      </c>
+      <c r="V63" s="101">
+        <v>20.193314999999998</v>
+      </c>
+    </row>
+    <row r="64" spans="2:22">
+      <c r="B64" s="109" t="s">
+        <v>207</v>
+      </c>
+      <c r="C64" s="101">
+        <v>4.8615060000000003</v>
+      </c>
+      <c r="D64" s="101">
+        <v>3.726315</v>
+      </c>
+      <c r="E64" s="101">
+        <v>1.5177750000000001</v>
+      </c>
+      <c r="F64" s="101">
+        <v>3.3705379999999998</v>
+      </c>
+      <c r="G64" s="101">
+        <v>4.7486069999999998</v>
+      </c>
+      <c r="H64" s="101">
+        <v>4.5395250000000003</v>
+      </c>
+      <c r="I64" s="101">
+        <v>4.2389780000000004</v>
+      </c>
+      <c r="J64" s="101">
+        <v>3.4370440000000002</v>
+      </c>
+      <c r="K64" s="101">
+        <v>3.5268190000000001</v>
+      </c>
+      <c r="L64" s="101">
+        <v>7.8388419999999996</v>
+      </c>
+      <c r="M64" s="101">
+        <v>9.5407580000000003</v>
+      </c>
+      <c r="N64" s="101">
+        <v>9.3683759999999996</v>
+      </c>
+      <c r="O64" s="101">
+        <v>8.1623140000000003</v>
+      </c>
+      <c r="P64" s="101">
+        <v>7.8205270000000002</v>
+      </c>
+      <c r="Q64" s="101">
+        <v>8.7740810000000007</v>
+      </c>
+      <c r="R64" s="101">
+        <v>9.8980800000000002</v>
+      </c>
+      <c r="S64" s="101">
+        <v>10.102183999999999</v>
+      </c>
+      <c r="T64" s="101">
+        <v>10.737242999999999</v>
+      </c>
+      <c r="U64" s="101">
+        <v>11.528843</v>
+      </c>
+      <c r="V64" s="101">
+        <v>11.604009</v>
+      </c>
+    </row>
+    <row r="65" spans="1:22">
+      <c r="B65" s="109" t="s">
+        <v>208</v>
+      </c>
+      <c r="C65" s="101">
+        <v>6.2002839999999999</v>
+      </c>
+      <c r="D65" s="101">
+        <v>4.6438560000000004</v>
+      </c>
+      <c r="E65" s="101">
+        <v>4.120425</v>
+      </c>
+      <c r="F65" s="101">
+        <v>3.134055</v>
+      </c>
+      <c r="G65" s="101">
+        <v>2.748329</v>
+      </c>
+      <c r="H65" s="101">
+        <v>6.2293950000000002</v>
+      </c>
+      <c r="I65" s="101">
+        <v>5.5224520000000004</v>
+      </c>
+      <c r="J65" s="101">
+        <v>3.3651300000000002</v>
+      </c>
+      <c r="K65" s="101">
+        <v>6.0459759999999996</v>
+      </c>
+      <c r="L65" s="101">
+        <v>5.6855330000000004</v>
+      </c>
+      <c r="M65" s="101">
+        <v>10.598985000000001</v>
+      </c>
+      <c r="N65" s="101">
+        <v>9.7700300000000002</v>
+      </c>
+      <c r="O65" s="101">
+        <v>7.4395829999999998</v>
+      </c>
+      <c r="P65" s="101">
+        <v>9.5389579999999992</v>
+      </c>
+      <c r="Q65" s="101">
+        <v>9.6084099999999992</v>
+      </c>
+      <c r="R65" s="101">
+        <v>11.271682999999999</v>
+      </c>
+      <c r="S65" s="101">
+        <v>11.952992999999999</v>
+      </c>
+      <c r="T65" s="101">
+        <v>15.032769</v>
+      </c>
+      <c r="U65" s="101">
+        <v>16.767455000000002</v>
+      </c>
+      <c r="V65" s="101">
+        <v>17.643588000000001</v>
+      </c>
+    </row>
+    <row r="66" spans="1:22">
+      <c r="B66" s="109" t="s">
+        <v>209</v>
+      </c>
+      <c r="C66" s="101">
+        <v>27.372159</v>
+      </c>
+      <c r="D66" s="101">
+        <v>34.621634</v>
+      </c>
+      <c r="E66" s="101">
+        <v>37.099567</v>
+      </c>
+      <c r="F66" s="101">
+        <v>42.886657</v>
+      </c>
+      <c r="G66" s="101">
+        <v>42.829704999999997</v>
+      </c>
+      <c r="H66" s="101">
+        <v>42.259801000000003</v>
+      </c>
+      <c r="I66" s="101">
+        <v>45.973990999999998</v>
+      </c>
+      <c r="J66" s="101">
+        <v>48.728822999999998</v>
+      </c>
+      <c r="K66" s="101">
+        <v>45.953823999999997</v>
+      </c>
+      <c r="L66" s="101">
+        <v>43.102499000000002</v>
+      </c>
+      <c r="M66" s="101">
+        <v>33.083308000000002</v>
+      </c>
+      <c r="N66" s="101">
+        <v>35.434505999999999</v>
+      </c>
+      <c r="O66" s="101">
+        <v>41.122202000000001</v>
+      </c>
+      <c r="P66" s="101">
+        <v>41.020955999999998</v>
+      </c>
+      <c r="Q66" s="101">
+        <v>39.011172999999999</v>
+      </c>
+      <c r="R66" s="101">
+        <v>35.511139</v>
+      </c>
+      <c r="S66" s="101">
+        <v>28.93252</v>
+      </c>
+      <c r="T66" s="101">
+        <v>27.640864000000001</v>
+      </c>
+      <c r="U66" s="101">
+        <v>24.967200999999999</v>
+      </c>
+      <c r="V66" s="101">
+        <v>25.301928</v>
+      </c>
+    </row>
+    <row r="67" spans="1:22">
+      <c r="B67" s="109" t="s">
+        <v>210</v>
+      </c>
+      <c r="C67" s="101">
+        <v>19.393939</v>
+      </c>
+      <c r="D67" s="101">
+        <v>16.225418999999999</v>
+      </c>
+      <c r="E67" s="101">
+        <v>14.546766</v>
+      </c>
+      <c r="F67" s="101">
+        <v>9.5308010000000003</v>
+      </c>
+      <c r="G67" s="101">
+        <v>6.5328090000000003</v>
+      </c>
+      <c r="H67" s="101">
+        <v>6.6219200000000003</v>
+      </c>
+      <c r="I67" s="101">
+        <v>6.1692869999999997</v>
+      </c>
+      <c r="J67" s="101">
+        <v>5.7985569999999997</v>
+      </c>
+      <c r="K67" s="101">
+        <v>8.4910099999999993</v>
+      </c>
+      <c r="L67" s="101">
+        <v>6.7305549999999998</v>
+      </c>
+      <c r="M67" s="101">
+        <v>7.9295309999999999</v>
+      </c>
+      <c r="N67" s="101">
+        <v>9.1903349999999993</v>
+      </c>
+      <c r="O67" s="101">
+        <v>9.1728970000000007</v>
+      </c>
+      <c r="P67" s="101">
+        <v>7.4540569999999997</v>
+      </c>
+      <c r="Q67" s="101">
+        <v>9.1073939999999993</v>
+      </c>
+      <c r="R67" s="101">
+        <v>9.5381699999999991</v>
+      </c>
+      <c r="S67" s="101">
+        <v>12.234508</v>
+      </c>
+      <c r="T67" s="101">
+        <v>14.828619</v>
+      </c>
+      <c r="U67" s="101">
+        <v>13.290763</v>
+      </c>
+      <c r="V67" s="101">
+        <v>12.93585</v>
+      </c>
+    </row>
+    <row r="68" spans="1:22">
+      <c r="B68" s="107"/>
+      <c r="C68" s="101"/>
+      <c r="D68" s="101"/>
+      <c r="E68" s="101"/>
+      <c r="F68" s="101"/>
+      <c r="G68" s="101"/>
+      <c r="H68" s="101"/>
+      <c r="I68" s="101"/>
+      <c r="J68" s="101"/>
+      <c r="K68" s="101"/>
+      <c r="L68" s="101"/>
+      <c r="M68" s="101"/>
+      <c r="N68" s="101"/>
+      <c r="O68" s="101"/>
+      <c r="P68" s="101"/>
+      <c r="Q68" s="101"/>
+      <c r="R68" s="101"/>
+      <c r="S68" s="101"/>
+      <c r="T68" s="101"/>
+      <c r="U68" s="101"/>
+      <c r="V68" s="101"/>
+    </row>
+    <row r="69" spans="1:22" ht="26.25">
+      <c r="A69" s="15"/>
+      <c r="B69" s="99" t="s">
+        <v>326</v>
+      </c>
+      <c r="C69" s="65">
+        <v>78.090522000000007</v>
+      </c>
+      <c r="D69" s="65">
+        <v>78.090522000000007</v>
+      </c>
+      <c r="E69" s="65">
+        <v>78.090522000000007</v>
+      </c>
+      <c r="F69" s="65">
+        <v>78.090522000000007</v>
+      </c>
+      <c r="G69" s="65">
+        <v>78.090522000000007</v>
+      </c>
+      <c r="H69" s="65">
+        <v>78.090522000000007</v>
+      </c>
+      <c r="I69" s="65">
+        <v>78.090522000000007</v>
+      </c>
+      <c r="J69" s="65">
+        <v>78.090522000000007</v>
+      </c>
+      <c r="K69" s="65">
+        <v>78.090522000000007</v>
+      </c>
+      <c r="L69" s="65">
+        <v>78.090522000000007</v>
+      </c>
+      <c r="M69" s="65">
+        <v>78.090522000000007</v>
+      </c>
+      <c r="N69" s="65">
+        <v>78.090522000000007</v>
+      </c>
+      <c r="O69" s="65">
+        <v>78.090522000000007</v>
+      </c>
+      <c r="P69" s="65">
+        <v>78.090522000000007</v>
+      </c>
+      <c r="Q69" s="65">
+        <v>78.090522000000007</v>
+      </c>
+      <c r="R69" s="65">
+        <v>78.090522000000007</v>
+      </c>
+      <c r="S69" s="65">
+        <v>78.090522000000007</v>
+      </c>
+      <c r="T69" s="65">
+        <v>78.090522000000007</v>
+      </c>
+      <c r="U69" s="65">
+        <v>78.090522000000007</v>
+      </c>
+      <c r="V69" s="65">
+        <v>78.090522000000007</v>
+      </c>
+    </row>
+    <row r="70" spans="1:22" ht="26.25">
+      <c r="B70" s="99" t="s">
+        <v>327</v>
+      </c>
+      <c r="C70" s="65">
+        <v>78.090522000000007</v>
+      </c>
+      <c r="D70" s="65">
+        <v>78.090522000000007</v>
+      </c>
+      <c r="E70" s="65">
+        <v>78.090522000000007</v>
+      </c>
+      <c r="F70" s="65">
+        <v>78.090522000000007</v>
+      </c>
+      <c r="G70" s="65">
+        <v>78.090522000000007</v>
+      </c>
+      <c r="H70" s="65">
+        <v>78.090522000000007</v>
+      </c>
+      <c r="I70" s="65">
+        <v>78.090522000000007</v>
+      </c>
+      <c r="J70" s="65">
+        <v>78.090522000000007</v>
+      </c>
+      <c r="K70" s="65">
+        <v>78.090522000000007</v>
+      </c>
+      <c r="L70" s="65">
+        <v>78.090522000000007</v>
+      </c>
+      <c r="M70" s="65">
+        <v>78.090522000000007</v>
+      </c>
+      <c r="N70" s="65">
+        <v>78.090522000000007</v>
+      </c>
+      <c r="O70" s="65">
+        <v>78.090522000000007</v>
+      </c>
+      <c r="P70" s="65">
+        <v>78.090522000000007</v>
+      </c>
+      <c r="Q70" s="65">
+        <v>78.090522000000007</v>
+      </c>
+      <c r="R70" s="65">
+        <v>78.090522000000007</v>
+      </c>
+      <c r="S70" s="65">
+        <v>78.090522000000007</v>
+      </c>
+      <c r="T70" s="65">
+        <v>78.090522000000007</v>
+      </c>
+      <c r="U70" s="65">
+        <v>78.090522000000007</v>
+      </c>
+      <c r="V70" s="65">
+        <v>78.090522000000007</v>
+      </c>
+    </row>
+    <row r="71" spans="1:22">
+      <c r="B71" s="99"/>
+    </row>
+    <row r="72" spans="1:22">
+      <c r="A72" s="12" t="s">
+        <v>328</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0B00-000000000000}">
   <sheetPr>
     <tabColor theme="3"/>
   </sheetPr>
   <dimension ref="A1:H7"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+    <sheetView topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2:H7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -32222,14 +36235,17 @@
       <c r="B5" s="58">
         <v>1.2405209526886144E-3</v>
       </c>
-      <c r="C5" s="58">
-        <v>4.2438874697242065E-4</v>
-      </c>
-      <c r="D5" s="58">
-        <v>4.2438874697242065E-4</v>
+      <c r="C5" s="60">
+        <f>D5</f>
+        <v>4.511510075790323E-4</v>
+      </c>
+      <c r="D5" s="60">
+        <f>E5</f>
+        <v>4.511510075790323E-4</v>
       </c>
       <c r="E5" s="60">
-        <v>4.2438874697242065E-4</v>
+        <f>'rail calcs'!C19</f>
+        <v>4.511510075790323E-4</v>
       </c>
       <c r="F5" s="58">
         <v>0</v>
@@ -32299,15 +36315,15 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0C00-000000000000}">
   <sheetPr>
     <tabColor theme="3"/>
   </sheetPr>
   <dimension ref="A1:H14"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F9" sqref="F9"/>
+    <sheetView topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2:H7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -32439,14 +36455,17 @@
       <c r="B5" s="58">
         <v>1.1140743815291445E-2</v>
       </c>
-      <c r="C5" s="58">
-        <v>3.4668839999999999E-3</v>
-      </c>
-      <c r="D5" s="58">
-        <v>3.4668839999999999E-3</v>
+      <c r="C5" s="60">
+        <f>D5</f>
+        <v>2.7959561517409449E-3</v>
+      </c>
+      <c r="D5" s="60">
+        <f>E5</f>
+        <v>2.7959561517409449E-3</v>
       </c>
       <c r="E5" s="60">
-        <v>3.4668839999999999E-3</v>
+        <f>'rail calcs'!C13</f>
+        <v>2.7959561517409449E-3</v>
       </c>
       <c r="F5" s="58">
         <v>0</v>
@@ -35604,12 +39623,6 @@
     </row>
   </sheetData>
   <mergeCells count="13">
-    <mergeCell ref="A45:B45"/>
-    <mergeCell ref="A8:B8"/>
-    <mergeCell ref="A9:B9"/>
-    <mergeCell ref="A30:B30"/>
-    <mergeCell ref="A42:B42"/>
-    <mergeCell ref="A44:B44"/>
     <mergeCell ref="A52:B52"/>
     <mergeCell ref="A46:B46"/>
     <mergeCell ref="A47:B47"/>
@@ -35617,6 +39630,12 @@
     <mergeCell ref="A49:B49"/>
     <mergeCell ref="A50:B50"/>
     <mergeCell ref="A51:B51"/>
+    <mergeCell ref="A45:B45"/>
+    <mergeCell ref="A8:B8"/>
+    <mergeCell ref="A9:B9"/>
+    <mergeCell ref="A30:B30"/>
+    <mergeCell ref="A42:B42"/>
+    <mergeCell ref="A44:B44"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="5" scale="50" fitToHeight="1000" orientation="landscape" r:id="rId1"/>
@@ -38433,11 +42452,6 @@
     </row>
   </sheetData>
   <mergeCells count="15">
-    <mergeCell ref="A39:B39"/>
-    <mergeCell ref="A7:B7"/>
-    <mergeCell ref="A8:B8"/>
-    <mergeCell ref="A9:B9"/>
-    <mergeCell ref="A29:B29"/>
     <mergeCell ref="A47:B47"/>
     <mergeCell ref="A48:B48"/>
     <mergeCell ref="A49:B49"/>
@@ -38448,6 +42462,11 @@
     <mergeCell ref="A44:B44"/>
     <mergeCell ref="A45:B45"/>
     <mergeCell ref="A46:B46"/>
+    <mergeCell ref="A39:B39"/>
+    <mergeCell ref="A7:B7"/>
+    <mergeCell ref="A8:B8"/>
+    <mergeCell ref="A9:B9"/>
+    <mergeCell ref="A29:B29"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="B6" r:id="rId1" xr:uid="{4215E112-E9B1-4A1C-AA81-ED2108378386}"/>
@@ -43322,10 +47341,10 @@
       <c r="AC2" s="32"/>
     </row>
     <row r="5" spans="1:32" ht="18" customHeight="1">
-      <c r="A5" s="98" t="s">
+      <c r="A5" s="96" t="s">
         <v>187</v>
       </c>
-      <c r="B5" s="98"/>
+      <c r="B5" s="96"/>
       <c r="C5" s="38"/>
       <c r="D5" s="38"/>
       <c r="E5" s="38"/>
@@ -48686,8 +52705,8 @@
       <c r="AF80" s="38"/>
     </row>
     <row r="81" spans="1:32" ht="14.65" customHeight="1">
-      <c r="A81" s="96"/>
-      <c r="B81" s="96"/>
+      <c r="A81" s="98"/>
+      <c r="B81" s="98"/>
       <c r="C81" s="15"/>
       <c r="D81" s="15"/>
       <c r="E81" s="15"/>
@@ -54441,6 +58460,37 @@
     </row>
   </sheetData>
   <mergeCells count="43">
+    <mergeCell ref="A156:B156"/>
+    <mergeCell ref="A125:B125"/>
+    <mergeCell ref="A133:B133"/>
+    <mergeCell ref="A136:B136"/>
+    <mergeCell ref="A138:B138"/>
+    <mergeCell ref="A139:B139"/>
+    <mergeCell ref="A148:B148"/>
+    <mergeCell ref="A116:B116"/>
+    <mergeCell ref="A81:B81"/>
+    <mergeCell ref="A82:B82"/>
+    <mergeCell ref="A95:B95"/>
+    <mergeCell ref="A107:B107"/>
+    <mergeCell ref="A109:B109"/>
+    <mergeCell ref="A110:B110"/>
+    <mergeCell ref="A111:B111"/>
+    <mergeCell ref="A112:B112"/>
+    <mergeCell ref="A113:B113"/>
+    <mergeCell ref="A114:B114"/>
+    <mergeCell ref="A115:B115"/>
+    <mergeCell ref="A79:B79"/>
+    <mergeCell ref="A31:B31"/>
+    <mergeCell ref="A38:B38"/>
+    <mergeCell ref="A44:B44"/>
+    <mergeCell ref="A46:B46"/>
+    <mergeCell ref="A47:B47"/>
+    <mergeCell ref="A48:B48"/>
+    <mergeCell ref="A49:B49"/>
+    <mergeCell ref="A50:B50"/>
+    <mergeCell ref="A51:B51"/>
+    <mergeCell ref="A64:B64"/>
+    <mergeCell ref="A76:B76"/>
     <mergeCell ref="A30:B30"/>
     <mergeCell ref="A5:B5"/>
     <mergeCell ref="A6:B6"/>
@@ -54453,37 +58503,6 @@
     <mergeCell ref="A19:B19"/>
     <mergeCell ref="A25:B25"/>
     <mergeCell ref="A28:B28"/>
-    <mergeCell ref="A79:B79"/>
-    <mergeCell ref="A31:B31"/>
-    <mergeCell ref="A38:B38"/>
-    <mergeCell ref="A44:B44"/>
-    <mergeCell ref="A46:B46"/>
-    <mergeCell ref="A47:B47"/>
-    <mergeCell ref="A48:B48"/>
-    <mergeCell ref="A49:B49"/>
-    <mergeCell ref="A50:B50"/>
-    <mergeCell ref="A51:B51"/>
-    <mergeCell ref="A64:B64"/>
-    <mergeCell ref="A76:B76"/>
-    <mergeCell ref="A116:B116"/>
-    <mergeCell ref="A81:B81"/>
-    <mergeCell ref="A82:B82"/>
-    <mergeCell ref="A95:B95"/>
-    <mergeCell ref="A107:B107"/>
-    <mergeCell ref="A109:B109"/>
-    <mergeCell ref="A110:B110"/>
-    <mergeCell ref="A111:B111"/>
-    <mergeCell ref="A112:B112"/>
-    <mergeCell ref="A113:B113"/>
-    <mergeCell ref="A114:B114"/>
-    <mergeCell ref="A115:B115"/>
-    <mergeCell ref="A156:B156"/>
-    <mergeCell ref="A125:B125"/>
-    <mergeCell ref="A133:B133"/>
-    <mergeCell ref="A136:B136"/>
-    <mergeCell ref="A138:B138"/>
-    <mergeCell ref="A139:B139"/>
-    <mergeCell ref="A148:B148"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -57660,11 +61679,12 @@
     </row>
   </sheetData>
   <mergeCells count="23">
-    <mergeCell ref="A59:B59"/>
-    <mergeCell ref="A60:B60"/>
-    <mergeCell ref="A61:B61"/>
-    <mergeCell ref="A62:B62"/>
-    <mergeCell ref="A63:B63"/>
+    <mergeCell ref="A37:B37"/>
+    <mergeCell ref="A5:B5"/>
+    <mergeCell ref="A6:B6"/>
+    <mergeCell ref="A7:B7"/>
+    <mergeCell ref="A8:B8"/>
+    <mergeCell ref="A9:B9"/>
     <mergeCell ref="A58:B58"/>
     <mergeCell ref="A47:B47"/>
     <mergeCell ref="A48:B48"/>
@@ -57677,12 +61697,11 @@
     <mergeCell ref="A55:B55"/>
     <mergeCell ref="A56:B56"/>
     <mergeCell ref="A57:B57"/>
-    <mergeCell ref="A37:B37"/>
-    <mergeCell ref="A5:B5"/>
-    <mergeCell ref="A6:B6"/>
-    <mergeCell ref="A7:B7"/>
-    <mergeCell ref="A8:B8"/>
-    <mergeCell ref="A9:B9"/>
+    <mergeCell ref="A59:B59"/>
+    <mergeCell ref="A60:B60"/>
+    <mergeCell ref="A61:B61"/>
+    <mergeCell ref="A62:B62"/>
+    <mergeCell ref="A63:B63"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -57690,12 +61709,23 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <of2ed5e60f3c4f8984f283882cb94320 xmlns="52604411-7aeb-406e-8b34-4ce79a7293cc">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </of2ed5e60f3c4f8984f283882cb94320>
+    <ff7c4ad8664a4671b57370e258acad6a xmlns="52604411-7aeb-406e-8b34-4ce79a7293cc">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </ff7c4ad8664a4671b57370e258acad6a>
+    <l787e5950a9249679d0130235a9a791b xmlns="52604411-7aeb-406e-8b34-4ce79a7293cc">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </l787e5950a9249679d0130235a9a791b>
+    <TaxCatchAll xmlns="52604411-7aeb-406e-8b34-4ce79a7293cc" xsi:nil="true"/>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="de340059-046a-4f1a-8b62-ade039df3700">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+  </documentManagement>
+</p:properties>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -57959,29 +61989,21 @@
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <of2ed5e60f3c4f8984f283882cb94320 xmlns="52604411-7aeb-406e-8b34-4ce79a7293cc">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </of2ed5e60f3c4f8984f283882cb94320>
-    <ff7c4ad8664a4671b57370e258acad6a xmlns="52604411-7aeb-406e-8b34-4ce79a7293cc">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </ff7c4ad8664a4671b57370e258acad6a>
-    <l787e5950a9249679d0130235a9a791b xmlns="52604411-7aeb-406e-8b34-4ce79a7293cc">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </l787e5950a9249679d0130235a9a791b>
-    <TaxCatchAll xmlns="52604411-7aeb-406e-8b34-4ce79a7293cc" xsi:nil="true"/>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="de340059-046a-4f1a-8b62-ade039df3700">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-  </documentManagement>
-</p:properties>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C9D73F77-AB54-4E48-8354-CA6FB71EB254}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0BB40CC4-551F-4602-B09A-217576ED5767}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="52604411-7aeb-406e-8b34-4ce79a7293cc"/>
+    <ds:schemaRef ds:uri="de340059-046a-4f1a-8b62-ade039df3700"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -58007,12 +62029,9 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0BB40CC4-551F-4602-B09A-217576ED5767}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C9D73F77-AB54-4E48-8354-CA6FB71EB254}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="52604411-7aeb-406e-8b34-4ce79a7293cc"/>
-    <ds:schemaRef ds:uri="de340059-046a-4f1a-8b62-ade039df3700"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>